<commit_message>
added disposalexpansioncost, storageexpansioncost, disposalexpansionleadtime, storageexpansionleadtime
</commit_message>
<xml_diff>
--- a/backend/app/internal/assets/pareto_input_template.xlsx
+++ b/backend/app/internal/assets/pareto_input_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelpesce/Desktop/pareto-ui/backend/app/internal/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62DEE77B-1393-2145-B16A-AAD8EA366940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CC11817-524A-2A40-AE5C-AAF90F6D3C42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19420" tabRatio="953" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19420" tabRatio="953" firstSheet="86" activeTab="91" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -134,7 +134,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="801" uniqueCount="264">
   <si>
     <t>Data Input Spreadsheet Overview</t>
   </si>
@@ -1863,7 +1863,7 @@
   </sheetPr>
   <dimension ref="B1:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
@@ -14243,7 +14243,9 @@
   </sheetPr>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -14261,18 +14263,10 @@
       <c r="A2" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>135</v>
-      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
@@ -14435,18 +14429,10 @@
       <c r="A2" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>125</v>
-      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
@@ -16493,12 +16479,8 @@
       <c r="A2" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>133</v>
-      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
     </row>
     <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
@@ -16522,7 +16504,7 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -16538,18 +16520,10 @@
       <c r="A2" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>125</v>
-      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>

</xml_diff>

<commit_message>
added disposalcapacityincrements, storagecapacityincrements, pipelinecapacityincrements
</commit_message>
<xml_diff>
--- a/backend/app/internal/assets/pareto_input_template.xlsx
+++ b/backend/app/internal/assets/pareto_input_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelpesce/Desktop/pareto-ui/backend/app/internal/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CC11817-524A-2A40-AE5C-AAF90F6D3C42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21551ACD-60D4-4446-ACF4-FB7A9660B163}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19420" tabRatio="953" firstSheet="86" activeTab="91" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19420" tabRatio="953" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -134,7 +134,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="801" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="264">
   <si>
     <t>Data Input Spreadsheet Overview</t>
   </si>
@@ -1010,7 +1010,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1035,14 +1035,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFCE4D6"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="26">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -1194,19 +1188,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -1337,7 +1318,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1403,47 +1384,47 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
@@ -1456,13 +1437,7 @@
     <xf numFmtId="3" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="9" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="9" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1484,6 +1459,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1863,7 +1847,7 @@
   </sheetPr>
   <dimension ref="B1:M37"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
@@ -7837,50 +7821,50 @@
       <c r="P2" s="7"/>
       <c r="Q2" s="7"/>
       <c r="R2" s="7"/>
-      <c r="S2" s="60"/>
-      <c r="T2" s="60"/>
-      <c r="U2" s="60"/>
-      <c r="V2" s="60"/>
-      <c r="W2" s="60"/>
-      <c r="X2" s="60"/>
-      <c r="Y2" s="60"/>
-      <c r="Z2" s="60"/>
-      <c r="AA2" s="60"/>
-      <c r="AB2" s="60"/>
-      <c r="AC2" s="60"/>
-      <c r="AD2" s="60"/>
-      <c r="AE2" s="60"/>
-      <c r="AF2" s="60"/>
-      <c r="AG2" s="60"/>
-      <c r="AH2" s="60"/>
-      <c r="AI2" s="60"/>
-      <c r="AJ2" s="60"/>
-      <c r="AK2" s="60"/>
-      <c r="AL2" s="60"/>
-      <c r="AM2" s="60"/>
-      <c r="AN2" s="60"/>
-      <c r="AO2" s="60"/>
-      <c r="AP2" s="60"/>
-      <c r="AQ2" s="60"/>
-      <c r="AR2" s="60"/>
-      <c r="AS2" s="60"/>
-      <c r="AT2" s="60"/>
-      <c r="AU2" s="60"/>
-      <c r="AV2" s="60"/>
-      <c r="AW2" s="60"/>
-      <c r="AX2" s="60"/>
-      <c r="AY2" s="60"/>
-      <c r="AZ2" s="60"/>
-      <c r="BA2" s="60"/>
-      <c r="BB2" s="60"/>
-      <c r="BC2" s="60"/>
-      <c r="BD2" s="60"/>
-      <c r="BE2" s="60"/>
-      <c r="BF2" s="60"/>
-      <c r="BG2" s="60"/>
-      <c r="BH2" s="60"/>
-      <c r="BI2" s="60"/>
-      <c r="BJ2" s="60"/>
+      <c r="S2" s="58"/>
+      <c r="T2" s="58"/>
+      <c r="U2" s="58"/>
+      <c r="V2" s="58"/>
+      <c r="W2" s="58"/>
+      <c r="X2" s="58"/>
+      <c r="Y2" s="58"/>
+      <c r="Z2" s="58"/>
+      <c r="AA2" s="58"/>
+      <c r="AB2" s="58"/>
+      <c r="AC2" s="58"/>
+      <c r="AD2" s="58"/>
+      <c r="AE2" s="58"/>
+      <c r="AF2" s="58"/>
+      <c r="AG2" s="58"/>
+      <c r="AH2" s="58"/>
+      <c r="AI2" s="58"/>
+      <c r="AJ2" s="58"/>
+      <c r="AK2" s="58"/>
+      <c r="AL2" s="58"/>
+      <c r="AM2" s="58"/>
+      <c r="AN2" s="58"/>
+      <c r="AO2" s="58"/>
+      <c r="AP2" s="58"/>
+      <c r="AQ2" s="58"/>
+      <c r="AR2" s="58"/>
+      <c r="AS2" s="58"/>
+      <c r="AT2" s="58"/>
+      <c r="AU2" s="58"/>
+      <c r="AV2" s="58"/>
+      <c r="AW2" s="58"/>
+      <c r="AX2" s="58"/>
+      <c r="AY2" s="58"/>
+      <c r="AZ2" s="58"/>
+      <c r="BA2" s="58"/>
+      <c r="BB2" s="58"/>
+      <c r="BC2" s="58"/>
+      <c r="BD2" s="58"/>
+      <c r="BE2" s="58"/>
+      <c r="BF2" s="58"/>
+      <c r="BG2" s="58"/>
+      <c r="BH2" s="58"/>
+      <c r="BI2" s="58"/>
+      <c r="BJ2" s="58"/>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
@@ -9227,7 +9211,7 @@
       <c r="BJ23" s="5"/>
     </row>
     <row r="24" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A24" s="61"/>
+      <c r="A24" s="59"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
@@ -9291,7 +9275,7 @@
       <c r="BJ24" s="5"/>
     </row>
     <row r="25" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A25" s="61"/>
+      <c r="A25" s="59"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
@@ -9355,7 +9339,7 @@
       <c r="BJ25" s="5"/>
     </row>
     <row r="26" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A26" s="61"/>
+      <c r="A26" s="59"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
@@ -9419,7 +9403,7 @@
       <c r="BJ26" s="5"/>
     </row>
     <row r="27" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A27" s="61"/>
+      <c r="A27" s="59"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
@@ -9483,7 +9467,7 @@
       <c r="BJ27" s="5"/>
     </row>
     <row r="28" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A28" s="61"/>
+      <c r="A28" s="59"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
@@ -9547,7 +9531,7 @@
       <c r="BJ28" s="5"/>
     </row>
     <row r="29" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A29" s="61"/>
+      <c r="A29" s="59"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
@@ -9611,7 +9595,7 @@
       <c r="BJ29" s="5"/>
     </row>
     <row r="30" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A30" s="61"/>
+      <c r="A30" s="59"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
@@ -9675,7 +9659,7 @@
       <c r="BJ30" s="5"/>
     </row>
     <row r="31" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A31" s="61"/>
+      <c r="A31" s="59"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
@@ -9739,7 +9723,7 @@
       <c r="BJ31" s="5"/>
     </row>
     <row r="32" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A32" s="61"/>
+      <c r="A32" s="59"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
@@ -9803,7 +9787,7 @@
       <c r="BJ32" s="5"/>
     </row>
     <row r="33" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A33" s="61"/>
+      <c r="A33" s="59"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
@@ -9867,7 +9851,7 @@
       <c r="BJ33" s="5"/>
     </row>
     <row r="34" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A34" s="61"/>
+      <c r="A34" s="59"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
@@ -9931,7 +9915,7 @@
       <c r="BJ34" s="5"/>
     </row>
     <row r="35" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A35" s="61"/>
+      <c r="A35" s="59"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
@@ -9995,7 +9979,7 @@
       <c r="BJ35" s="5"/>
     </row>
     <row r="36" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A36" s="61"/>
+      <c r="A36" s="59"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
@@ -10059,7 +10043,7 @@
       <c r="BJ36" s="5"/>
     </row>
     <row r="37" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A37" s="61"/>
+      <c r="A37" s="59"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
@@ -10123,7 +10107,7 @@
       <c r="BJ37" s="5"/>
     </row>
     <row r="38" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A38" s="61"/>
+      <c r="A38" s="59"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
@@ -10187,7 +10171,7 @@
       <c r="BJ38" s="5"/>
     </row>
     <row r="39" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A39" s="61"/>
+      <c r="A39" s="59"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
@@ -10251,7 +10235,7 @@
       <c r="BJ39" s="5"/>
     </row>
     <row r="40" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A40" s="61"/>
+      <c r="A40" s="59"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
@@ -10315,7 +10299,7 @@
       <c r="BJ40" s="5"/>
     </row>
     <row r="41" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A41" s="61"/>
+      <c r="A41" s="59"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
@@ -10379,7 +10363,7 @@
       <c r="BJ41" s="5"/>
     </row>
     <row r="42" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A42" s="61"/>
+      <c r="A42" s="59"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
@@ -10443,7 +10427,7 @@
       <c r="BJ42" s="5"/>
     </row>
     <row r="43" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A43" s="61"/>
+      <c r="A43" s="59"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
@@ -10507,7 +10491,7 @@
       <c r="BJ43" s="5"/>
     </row>
     <row r="44" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A44" s="61"/>
+      <c r="A44" s="59"/>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
@@ -10571,7 +10555,7 @@
       <c r="BJ44" s="5"/>
     </row>
     <row r="45" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A45" s="61"/>
+      <c r="A45" s="59"/>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
@@ -10635,7 +10619,7 @@
       <c r="BJ45" s="5"/>
     </row>
     <row r="46" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A46" s="61"/>
+      <c r="A46" s="59"/>
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
@@ -10699,7 +10683,7 @@
       <c r="BJ46" s="5"/>
     </row>
     <row r="47" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A47" s="61"/>
+      <c r="A47" s="59"/>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
@@ -10763,7 +10747,7 @@
       <c r="BJ47" s="5"/>
     </row>
     <row r="48" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A48" s="61"/>
+      <c r="A48" s="59"/>
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
@@ -10827,7 +10811,7 @@
       <c r="BJ48" s="5"/>
     </row>
     <row r="49" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A49" s="61"/>
+      <c r="A49" s="59"/>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
@@ -10891,7 +10875,7 @@
       <c r="BJ49" s="5"/>
     </row>
     <row r="50" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A50" s="61"/>
+      <c r="A50" s="59"/>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
@@ -10955,7 +10939,7 @@
       <c r="BJ50" s="5"/>
     </row>
     <row r="51" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A51" s="61"/>
+      <c r="A51" s="59"/>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
@@ -11019,7 +11003,7 @@
       <c r="BJ51" s="5"/>
     </row>
     <row r="52" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A52" s="61"/>
+      <c r="A52" s="59"/>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
@@ -11083,7 +11067,7 @@
       <c r="BJ52" s="5"/>
     </row>
     <row r="53" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A53" s="61"/>
+      <c r="A53" s="59"/>
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
@@ -11147,7 +11131,7 @@
       <c r="BJ53" s="5"/>
     </row>
     <row r="54" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A54" s="61"/>
+      <c r="A54" s="59"/>
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
@@ -11211,7 +11195,7 @@
       <c r="BJ54" s="5"/>
     </row>
     <row r="55" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A55" s="61"/>
+      <c r="A55" s="59"/>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
@@ -11275,7 +11259,7 @@
       <c r="BJ55" s="5"/>
     </row>
     <row r="56" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A56" s="61"/>
+      <c r="A56" s="59"/>
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
@@ -11339,7 +11323,7 @@
       <c r="BJ56" s="5"/>
     </row>
     <row r="57" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A57" s="61"/>
+      <c r="A57" s="59"/>
       <c r="B57" s="5"/>
       <c r="C57" s="5"/>
       <c r="D57" s="5"/>
@@ -11403,7 +11387,7 @@
       <c r="BJ57" s="5"/>
     </row>
     <row r="58" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A58" s="61"/>
+      <c r="A58" s="59"/>
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
@@ -11467,7 +11451,7 @@
       <c r="BJ58" s="5"/>
     </row>
     <row r="59" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A59" s="61"/>
+      <c r="A59" s="59"/>
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
       <c r="D59" s="5"/>
@@ -11531,7 +11515,7 @@
       <c r="BJ59" s="5"/>
     </row>
     <row r="60" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A60" s="61"/>
+      <c r="A60" s="59"/>
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
       <c r="D60" s="5"/>
@@ -11595,7 +11579,7 @@
       <c r="BJ60" s="5"/>
     </row>
     <row r="61" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A61" s="61"/>
+      <c r="A61" s="59"/>
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
@@ -11659,7 +11643,7 @@
       <c r="BJ61" s="5"/>
     </row>
     <row r="62" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A62" s="61"/>
+      <c r="A62" s="59"/>
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
@@ -11723,7 +11707,7 @@
       <c r="BJ62" s="5"/>
     </row>
     <row r="63" spans="1:62" x14ac:dyDescent="0.2">
-      <c r="A63" s="61"/>
+      <c r="A63" s="59"/>
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
@@ -14304,51 +14288,35 @@
     <col min="2" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Disposal Capacity Expansion Increments [",VLOOKUP("volume", Units!$A$2:$B$11, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$11, 2, FALSE),"]")</f>
         <v>Table of Disposal Capacity Expansion Increments [bbl/day]</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="66" t="s">
         <v>216</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="66" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="22" t="s">
-        <v>132</v>
-      </c>
-      <c r="B3" s="26">
-        <v>0</v>
-      </c>
+      <c r="A3" s="66"/>
+      <c r="B3" s="67"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="22" t="s">
-        <v>133</v>
-      </c>
-      <c r="B4" s="59">
-        <v>7143</v>
-      </c>
+      <c r="A4" s="66"/>
+      <c r="B4" s="68"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="22" t="s">
-        <v>134</v>
-      </c>
-      <c r="B5" s="59">
-        <v>14286</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="B6" s="58">
-        <v>50000</v>
-      </c>
+      <c r="A5" s="66"/>
+      <c r="B5" s="68"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="66"/>
+      <c r="B6" s="68"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14468,9 +14436,7 @@
   </sheetPr>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -14478,51 +14444,35 @@
     <col min="2" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Storage Capacity Expansion Increments [",VLOOKUP("volume", Units!$A$2:$B$11, 2, FALSE),"]")</f>
         <v>Table of Storage Capacity Expansion Increments [bbl]</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="66" t="s">
         <v>217</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="66" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="22" t="s">
-        <v>122</v>
-      </c>
-      <c r="B3" s="26">
-        <v>0</v>
-      </c>
+      <c r="A3" s="66"/>
+      <c r="B3" s="67"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="22" t="s">
-        <v>123</v>
-      </c>
-      <c r="B4" s="26">
-        <v>50000</v>
-      </c>
+      <c r="A4" s="66"/>
+      <c r="B4" s="67"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="22" t="s">
-        <v>124</v>
-      </c>
-      <c r="B5" s="26">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
-        <v>125</v>
-      </c>
-      <c r="B6" s="28">
-        <v>350000</v>
-      </c>
+      <c r="A5" s="66"/>
+      <c r="B5" s="67"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="66"/>
+      <c r="B6" s="67"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14702,13 +14652,13 @@
       <c r="A3" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="B3" s="65">
+      <c r="B3" s="63">
         <v>0</v>
       </c>
-      <c r="C3" s="65">
+      <c r="C3" s="63">
         <v>10000</v>
       </c>
-      <c r="D3" s="65">
+      <c r="D3" s="63">
         <v>20000</v>
       </c>
       <c r="E3" s="26">
@@ -14719,13 +14669,13 @@
       <c r="A4" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="B4" s="65">
+      <c r="B4" s="63">
         <v>0</v>
       </c>
-      <c r="C4" s="65">
+      <c r="C4" s="63">
         <v>10000</v>
       </c>
-      <c r="D4" s="65">
+      <c r="D4" s="63">
         <v>20000</v>
       </c>
       <c r="E4" s="26">
@@ -14736,13 +14686,13 @@
       <c r="A5" s="22" t="s">
         <v>235</v>
       </c>
-      <c r="B5" s="65">
+      <c r="B5" s="63">
         <v>0</v>
       </c>
-      <c r="C5" s="65">
+      <c r="C5" s="63">
         <v>10000</v>
       </c>
-      <c r="D5" s="65">
+      <c r="D5" s="63">
         <v>20000</v>
       </c>
       <c r="E5" s="26">
@@ -14996,8 +14946,8 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="7"/>
-      <c r="B8" s="64"/>
-      <c r="C8" s="64"/>
+      <c r="B8" s="62"/>
+      <c r="C8" s="62"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
@@ -15005,7 +14955,7 @@
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
-      <c r="K8" s="64"/>
+      <c r="K8" s="62"/>
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
@@ -15019,8 +14969,8 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="7"/>
-      <c r="B9" s="64"/>
-      <c r="C9" s="64"/>
+      <c r="B9" s="62"/>
+      <c r="C9" s="62"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
@@ -15089,7 +15039,7 @@
     <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
       <c r="B12" s="5"/>
-      <c r="C12" s="64"/>
+      <c r="C12" s="62"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
@@ -15412,7 +15362,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
-      <c r="B3" s="67"/>
+      <c r="B3" s="65"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -15421,7 +15371,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="7"/>
-      <c r="B4" s="67"/>
+      <c r="B4" s="65"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -15442,7 +15392,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15451,57 +15401,57 @@
     <col min="2" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="str">
         <f>_xlfn.CONCAT( "Table of Pipeline Capacity Expansion Increments [",VLOOKUP("volume", Units!$A$2:$B$11, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$11, 2, FALSE),"]")</f>
         <v>Table of Pipeline Capacity Expansion Increments [bbl/day]</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="66" t="s">
         <v>215</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="66" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="66" t="s">
         <v>116</v>
       </c>
-      <c r="B3" s="26">
+      <c r="B3" s="67">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="66" t="s">
         <v>117</v>
       </c>
-      <c r="B4" s="26">
+      <c r="B4" s="67">
         <v>14285.714285714286</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="66" t="s">
         <v>118</v>
       </c>
-      <c r="B5" s="26">
+      <c r="B5" s="67">
         <v>35714.285714285717</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="66" t="s">
         <v>119</v>
       </c>
-      <c r="B6" s="26">
+      <c r="B6" s="67">
         <v>42857.142857142855</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="23" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="66" t="s">
         <v>120</v>
       </c>
-      <c r="B7" s="28">
+      <c r="B7" s="67">
         <v>50000</v>
       </c>
     </row>
@@ -15864,7 +15814,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="66" t="s">
+      <c r="A6" s="64" t="s">
         <v>236</v>
       </c>
       <c r="B6" s="28">
@@ -16167,23 +16117,23 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
-      <c r="B3" s="63"/>
+      <c r="B3" s="61"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="7"/>
-      <c r="B4" s="63"/>
+      <c r="B4" s="61"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
-      <c r="B5" s="63"/>
+      <c r="B5" s="61"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="7"/>
-      <c r="B6" s="63"/>
+      <c r="B6" s="61"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
-      <c r="B7" s="63"/>
+      <c r="B7" s="61"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16223,15 +16173,15 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
-      <c r="B3" s="63"/>
+      <c r="B3" s="61"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="7"/>
-      <c r="B4" s="63"/>
+      <c r="B4" s="61"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
-      <c r="B5" s="63"/>
+      <c r="B5" s="61"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -16272,7 +16222,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
-      <c r="B3" s="63"/>
+      <c r="B3" s="61"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16504,7 +16454,7 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -16583,7 +16533,7 @@
       <c r="A3" s="23" t="s">
         <v>263</v>
       </c>
-      <c r="B3" s="62">
+      <c r="B3" s="60">
         <v>0.2</v>
       </c>
     </row>
@@ -16631,28 +16581,28 @@
     </row>
     <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
-      <c r="B3" s="67"/>
+      <c r="B3" s="65"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="7"/>
-      <c r="B4" s="67"/>
+      <c r="B4" s="65"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
-      <c r="B5" s="67"/>
+      <c r="B5" s="65"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="7"/>
-      <c r="B6" s="67"/>
+      <c r="B6" s="65"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>

</xml_diff>

<commit_message>
add column headers for those 2
</commit_message>
<xml_diff>
--- a/backend/app/internal/assets/pareto_input_template.xlsx
+++ b/backend/app/internal/assets/pareto_input_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelpesce/Desktop/pareto-ui/backend/app/internal/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAB89683-681B-714A-90FD-D5ECD00175B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04838C2B-2E3A-0C4E-A983-5E43E9F68399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19420" tabRatio="953" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
@@ -134,7 +134,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="264">
   <si>
     <t>Data Input Spreadsheet Overview</t>
   </si>
@@ -1307,7 +1307,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1436,12 +1436,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -14598,41 +14592,41 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="62"/>
-      <c r="B3" s="63"/>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="62"/>
-      <c r="B4" s="63"/>
-      <c r="C4" s="63"/>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="62"/>
-      <c r="B5" s="63"/>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
-      <c r="E5" s="63"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="62"/>
-      <c r="B6" s="63"/>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="54"/>
+      <c r="D6" s="54"/>
+      <c r="E6" s="54"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="6"/>
@@ -15262,21 +15256,11 @@
       <c r="B2" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>120</v>
-      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="6"/>
@@ -16294,6 +16278,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="str">
@@ -16335,6 +16322,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="str">
@@ -16447,15 +16437,9 @@
       <c r="B2" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>119</v>
-      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="6"/>

</xml_diff>

<commit_message>
update excel  template to remove VLOOKup breaking it
</commit_message>
<xml_diff>
--- a/backend/app/internal/assets/pareto_input_template.xlsx
+++ b/backend/app/internal/assets/pareto_input_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelpesce/Desktop/pareto-ui/backend/app/internal/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0546BD1-2ED2-A54D-B775-A13B8D3BAD92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A35B2066-22E2-6947-9679-4DF36C426259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19420" tabRatio="953" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="-35000" yWindow="500" windowWidth="34560" windowHeight="18980" tabRatio="953" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -111,9 +111,6 @@
     <sheet name="PipelineExpansionLeadTime_Dist" sheetId="131" r:id="rId96"/>
     <sheet name="PipelineExpansionLeadTime_Capac" sheetId="132" r:id="rId97"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId98"/>
-  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="76" hidden="1">#REF!</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">TreatmentTechnologies!$A$1:$A$5</definedName>
@@ -241,9 +238,6 @@
     <t>Cost for sourcing freshwater for frac</t>
   </si>
   <si>
-    <t>Figure 1: Illustration of the optimization workflow</t>
-  </si>
-  <si>
     <t>Reuse Costs</t>
   </si>
   <si>
@@ -938,6 +932,9 @@
   </si>
   <si>
     <t>Treatment Sites to Disposal Trucking Arcs (1 denotes an arc for the treated stream and 2 denotes an arc for the residual stream) [-]</t>
+  </si>
+  <si>
+    <t>Table with processing cost for sending water to beneficial reuse [USD/bbl]</t>
   </si>
 </sst>
 </file>
@@ -1319,7 +1316,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1450,9 +1447,6 @@
     <xf numFmtId="3" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -1477,344 +1471,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>503714</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>4946</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>404754</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>144522</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{087B3C07-F1EA-47EB-AEEC-96EF7CAC7D17}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6955974" y="1113310"/>
-          <a:ext cx="3166753" cy="4167290"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Overview"/>
-      <sheetName val="Schematic"/>
-      <sheetName val="Units"/>
-      <sheetName val="ProductionPads"/>
-      <sheetName val="ProductionTanks"/>
-      <sheetName val="CompletionsPads"/>
-      <sheetName val="SWDSites"/>
-      <sheetName val="FreshwaterSources"/>
-      <sheetName val="StorageSites"/>
-      <sheetName val="TreatmentSites"/>
-      <sheetName val="TreatmentTechnologies"/>
-      <sheetName val="ReuseOptions"/>
-      <sheetName val="NetworkNodes"/>
-      <sheetName val="PipelineDiameters"/>
-      <sheetName val="StorageCapacities"/>
-      <sheetName val="TreatmentCapacities"/>
-      <sheetName val="InjectionCapacities"/>
-      <sheetName val="PNA"/>
-      <sheetName val="CNA"/>
-      <sheetName val="CCA"/>
-      <sheetName val="NNA"/>
-      <sheetName val="NCA"/>
-      <sheetName val="NKA"/>
-      <sheetName val="NRA"/>
-      <sheetName val="NSA"/>
-      <sheetName val="NOA"/>
-      <sheetName val="SNA"/>
-      <sheetName val="SOA"/>
-      <sheetName val="FCA"/>
-      <sheetName val="RCA"/>
-      <sheetName val="RSA"/>
-      <sheetName val="SCA"/>
-      <sheetName val="RNA"/>
-      <sheetName val="ROA"/>
-      <sheetName val="RKA"/>
-      <sheetName val="PCT"/>
-      <sheetName val="FCT"/>
-      <sheetName val="PKT"/>
-      <sheetName val="CKT"/>
-      <sheetName val="CCT"/>
-      <sheetName val="CST"/>
-      <sheetName val="RST"/>
-      <sheetName val="ROT"/>
-      <sheetName val="SOT"/>
-      <sheetName val="RKT"/>
-      <sheetName val="Elevation"/>
-      <sheetName val="CompletionsDemand"/>
-      <sheetName val="PadRates"/>
-      <sheetName val="FlowbackRates"/>
-      <sheetName val="WellPressure"/>
-      <sheetName val="InitialPipelineCapacity"/>
-      <sheetName val="InitialPipelineDiameters"/>
-      <sheetName val="InitialDisposalCapacity"/>
-      <sheetName val="InitialStorageCapacity"/>
-      <sheetName val="InitialTreatmentCapacity"/>
-      <sheetName val="ReuseMinimum"/>
-      <sheetName val="ReuseCapacity"/>
-      <sheetName val="FreshwaterSourcingAvailability"/>
-      <sheetName val="CompletionsPadStorage"/>
-      <sheetName val="PadOffloadingCapacity"/>
-      <sheetName val="NodeCapacities"/>
-      <sheetName val="DisposalOperatingCapacity"/>
-      <sheetName val="DisposalOperationalCost"/>
-      <sheetName val="TreatmentOperationalCost"/>
-      <sheetName val="ReuseOperationalCost"/>
-      <sheetName val="PipelineOperationalCost"/>
-      <sheetName val="FreshSourcingCost"/>
-      <sheetName val="TruckingHourlyCost"/>
-      <sheetName val="TruckingTime"/>
-      <sheetName val="DisposalExpansionCost"/>
-      <sheetName val="DisposalCapacityIncrements"/>
-      <sheetName val="StorageExpansionCost"/>
-      <sheetName val="StorageCapacityIncrements"/>
-      <sheetName val="TreatmentExpansionCost"/>
-      <sheetName val="TreatmentCapacityIncrements"/>
-      <sheetName val="PipelineCapexDistanceBased"/>
-      <sheetName val="PipelineExpansionDistance"/>
-      <sheetName val="PipelineCapexCapacityBased"/>
-      <sheetName val="PipelineCapacityIncrements"/>
-      <sheetName val="PipelineDiameterValues"/>
-      <sheetName val="TreatmentEfficiency"/>
-      <sheetName val="RemovalEfficiency"/>
-      <sheetName val="DesalinationTechnologies"/>
-      <sheetName val="DesalinationSites"/>
-      <sheetName val="BeneficialReuseCost"/>
-      <sheetName val="BeneficialReuseCredit"/>
-      <sheetName val="CompletionsPadOutsideSystem"/>
-      <sheetName val="Hydraulics"/>
-      <sheetName val="Economics"/>
-      <sheetName val="PadWaterQuality"/>
-      <sheetName val="StorageInitialWaterQuality"/>
-      <sheetName val="PadStorageInitialWaterQuality"/>
-      <sheetName val="TreatmentExpansionLeadTime"/>
-      <sheetName val="DisposalExpansionLeadTime"/>
-      <sheetName val="StorageExpansionLeadTime"/>
-      <sheetName val="PipelineExpansionLeadTime_Dist"/>
-      <sheetName val="PipelineExpansionLeadTime_Capac"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2">
-        <row r="2">
-          <cell r="A2" t="str">
-            <v>INDEX</v>
-          </cell>
-          <cell r="B2" t="str">
-            <v>VALUE</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3" t="str">
-            <v>volume</v>
-          </cell>
-          <cell r="B3" t="str">
-            <v>bbl</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4" t="str">
-            <v>distance</v>
-          </cell>
-          <cell r="B4" t="str">
-            <v>mile</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5" t="str">
-            <v>diameter</v>
-          </cell>
-          <cell r="B5" t="str">
-            <v>inch</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6" t="str">
-            <v>concentration</v>
-          </cell>
-          <cell r="B6" t="str">
-            <v>mg/liter</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7" t="str">
-            <v>currency</v>
-          </cell>
-          <cell r="B7" t="str">
-            <v>USD</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8" t="str">
-            <v>time</v>
-          </cell>
-          <cell r="B8" t="str">
-            <v>day</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9" t="str">
-            <v>pressure</v>
-          </cell>
-          <cell r="B9" t="str">
-            <v>psi</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10" t="str">
-            <v>elevation</v>
-          </cell>
-          <cell r="B10" t="str">
-            <v>foot</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11" t="str">
-            <v>decision period</v>
-          </cell>
-          <cell r="B11" t="str">
-            <v>week</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
-      <sheetData sheetId="27"/>
-      <sheetData sheetId="28"/>
-      <sheetData sheetId="29"/>
-      <sheetData sheetId="30"/>
-      <sheetData sheetId="31"/>
-      <sheetData sheetId="32"/>
-      <sheetData sheetId="33"/>
-      <sheetData sheetId="34"/>
-      <sheetData sheetId="35"/>
-      <sheetData sheetId="36"/>
-      <sheetData sheetId="37"/>
-      <sheetData sheetId="38"/>
-      <sheetData sheetId="39"/>
-      <sheetData sheetId="40"/>
-      <sheetData sheetId="41"/>
-      <sheetData sheetId="42"/>
-      <sheetData sheetId="43"/>
-      <sheetData sheetId="44"/>
-      <sheetData sheetId="45"/>
-      <sheetData sheetId="46"/>
-      <sheetData sheetId="47"/>
-      <sheetData sheetId="48"/>
-      <sheetData sheetId="49"/>
-      <sheetData sheetId="50"/>
-      <sheetData sheetId="51"/>
-      <sheetData sheetId="52"/>
-      <sheetData sheetId="53"/>
-      <sheetData sheetId="54"/>
-      <sheetData sheetId="55"/>
-      <sheetData sheetId="56"/>
-      <sheetData sheetId="57"/>
-      <sheetData sheetId="58"/>
-      <sheetData sheetId="59"/>
-      <sheetData sheetId="60"/>
-      <sheetData sheetId="61"/>
-      <sheetData sheetId="62"/>
-      <sheetData sheetId="63"/>
-      <sheetData sheetId="64"/>
-      <sheetData sheetId="65"/>
-      <sheetData sheetId="66"/>
-      <sheetData sheetId="67"/>
-      <sheetData sheetId="68"/>
-      <sheetData sheetId="69"/>
-      <sheetData sheetId="70"/>
-      <sheetData sheetId="71"/>
-      <sheetData sheetId="72"/>
-      <sheetData sheetId="73"/>
-      <sheetData sheetId="74"/>
-      <sheetData sheetId="75"/>
-      <sheetData sheetId="76"/>
-      <sheetData sheetId="77"/>
-      <sheetData sheetId="78"/>
-      <sheetData sheetId="79"/>
-      <sheetData sheetId="80"/>
-      <sheetData sheetId="81"/>
-      <sheetData sheetId="82"/>
-      <sheetData sheetId="83"/>
-      <sheetData sheetId="84"/>
-      <sheetData sheetId="85"/>
-      <sheetData sheetId="86"/>
-      <sheetData sheetId="87"/>
-      <sheetData sheetId="88"/>
-      <sheetData sheetId="89"/>
-      <sheetData sheetId="90"/>
-      <sheetData sheetId="91"/>
-      <sheetData sheetId="92"/>
-      <sheetData sheetId="93"/>
-      <sheetData sheetId="94"/>
-      <sheetData sheetId="95"/>
-      <sheetData sheetId="96"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2119,9 +1775,7 @@
   </sheetPr>
   <dimension ref="B1:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2556,19 +2210,17 @@
       <c r="I31" s="12"/>
       <c r="J31" s="12"/>
       <c r="K31" s="13"/>
-      <c r="M31" s="19" t="s">
-        <v>33</v>
-      </c>
+      <c r="M31" s="19"/>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B32" s="10"/>
       <c r="C32" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D32" s="12"/>
       <c r="E32" s="12"/>
       <c r="F32" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G32" s="12"/>
       <c r="H32" s="12"/>
@@ -2579,12 +2231,12 @@
     <row r="33" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B33" s="10"/>
       <c r="C33" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D33" s="12"/>
       <c r="E33" s="12"/>
       <c r="F33" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G33" s="12"/>
       <c r="H33" s="12"/>
@@ -2595,12 +2247,12 @@
     <row r="34" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B34" s="10"/>
       <c r="C34" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D34" s="12"/>
       <c r="E34" s="12"/>
       <c r="F34" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G34" s="12"/>
       <c r="H34" s="12"/>
@@ -2611,12 +2263,12 @@
     <row r="35" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B35" s="10"/>
       <c r="C35" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D35" s="12"/>
       <c r="E35" s="12"/>
       <c r="F35" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G35" s="12"/>
       <c r="H35" s="12"/>
@@ -2627,12 +2279,12 @@
     <row r="36" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B36" s="10"/>
       <c r="C36" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D36" s="12"/>
       <c r="E36" s="12"/>
       <c r="F36" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G36" s="12"/>
       <c r="H36" s="12"/>
@@ -2670,7 +2322,6 @@
     <hyperlink ref="C36" location="PipelineCapexDistanceBased!A1" display="Pipeline Expansion" xr:uid="{71654592-CF02-4564-8F69-88D94B3F411B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2700,7 +2351,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
@@ -2757,17 +2408,17 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="N3" s="6"/>
       <c r="O3" s="6"/>
@@ -2775,12 +2426,12 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
@@ -2817,7 +2468,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
@@ -2864,7 +2515,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
@@ -2990,32 +2641,32 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -3050,17 +2701,17 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N3" s="6"/>
       <c r="O3" s="6"/>
@@ -3068,12 +2719,12 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
@@ -3114,17 +2765,17 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N3" s="6"/>
       <c r="O3" s="6"/>
@@ -3132,12 +2783,12 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
@@ -3178,17 +2829,17 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N3" s="6"/>
       <c r="O3" s="6"/>
@@ -3196,12 +2847,12 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
@@ -3235,12 +2886,12 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -3291,12 +2942,12 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -3412,12 +3063,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B2" s="6"/>
     </row>
@@ -3450,12 +3101,12 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -3574,12 +3225,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B2" s="6"/>
     </row>
@@ -3648,12 +3299,12 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -3734,12 +3385,12 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -3818,12 +3469,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -3906,12 +3557,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -3994,12 +3645,12 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -4070,12 +3721,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -4119,12 +3770,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B2" s="6"/>
     </row>
@@ -4178,21 +3829,21 @@
   <sheetData>
     <row r="1" spans="1:53" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:53" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="D2" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="D2" s="50" t="s">
+      <c r="E2" s="51" t="s">
         <v>47</v>
-      </c>
-      <c r="E2" s="51" t="s">
-        <v>48</v>
       </c>
       <c r="F2" s="43"/>
       <c r="G2" s="43"/>
@@ -4203,52 +3854,52 @@
     </row>
     <row r="3" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="D3" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="E3" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="E3" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="F3" s="40" t="s">
+      <c r="G3" s="33" t="s">
         <v>52</v>
-      </c>
-      <c r="G3" s="33" t="s">
-        <v>53</v>
       </c>
       <c r="H3" s="37"/>
       <c r="I3" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="J3" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="K3" s="35" t="s">
         <v>54</v>
-      </c>
-      <c r="J3" s="40" t="s">
-        <v>52</v>
-      </c>
-      <c r="K3" s="35" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A4" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="D4" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="D4" s="38" t="s">
+      <c r="E4" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="E4" s="39" t="s">
+      <c r="F4" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" s="33" t="s">
         <v>59</v>
-      </c>
-      <c r="F4" s="40" t="s">
-        <v>52</v>
-      </c>
-      <c r="G4" s="33" t="s">
-        <v>60</v>
       </c>
       <c r="H4" s="37"/>
       <c r="I4" s="33"/>
@@ -4257,13 +3908,13 @@
     </row>
     <row r="5" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A5" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="D5" s="38" t="s">
         <v>62</v>
-      </c>
-      <c r="D5" s="38" t="s">
-        <v>63</v>
       </c>
       <c r="E5" s="41"/>
       <c r="F5" s="34"/>
@@ -4275,22 +3926,22 @@
     </row>
     <row r="6" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A6" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="D6" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="D6" s="38" t="s">
+      <c r="E6" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" s="33" t="s">
         <v>66</v>
-      </c>
-      <c r="E6" s="39" t="s">
-        <v>65</v>
-      </c>
-      <c r="F6" s="40" t="s">
-        <v>52</v>
-      </c>
-      <c r="G6" s="33" t="s">
-        <v>67</v>
       </c>
       <c r="H6" s="38"/>
       <c r="I6" s="34"/>
@@ -4299,22 +3950,22 @@
     </row>
     <row r="7" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A7" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="D7" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="D7" s="38" t="s">
+      <c r="E7" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="E7" s="39" t="s">
+      <c r="F7" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" s="33" t="s">
         <v>71</v>
-      </c>
-      <c r="F7" s="40" t="s">
-        <v>52</v>
-      </c>
-      <c r="G7" s="33" t="s">
-        <v>72</v>
       </c>
       <c r="H7" s="38"/>
       <c r="I7" s="34"/>
@@ -4323,13 +3974,13 @@
     </row>
     <row r="8" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A8" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="D8" s="38" t="s">
         <v>74</v>
-      </c>
-      <c r="D8" s="38" t="s">
-        <v>75</v>
       </c>
       <c r="E8" s="41"/>
       <c r="F8" s="34"/>
@@ -4339,87 +3990,87 @@
       <c r="J8" s="34"/>
       <c r="K8" s="36"/>
       <c r="AT8" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AU8" s="24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AV8" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AW8" s="24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AX8" s="24" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AY8" s="24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AZ8" s="24" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="BA8" s="24" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A9" s="21" t="s">
+        <v>237</v>
+      </c>
+      <c r="B9" s="30" t="s">
         <v>238</v>
       </c>
-      <c r="B9" s="30" t="s">
+      <c r="D9" s="38" t="s">
         <v>239</v>
       </c>
-      <c r="D9" s="38" t="s">
+      <c r="E9" s="41" t="s">
+        <v>238</v>
+      </c>
+      <c r="F9" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="G9" s="34" t="s">
         <v>240</v>
-      </c>
-      <c r="E9" s="41" t="s">
-        <v>239</v>
-      </c>
-      <c r="F9" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="G9" s="34" t="s">
-        <v>241</v>
       </c>
       <c r="H9" s="38"/>
       <c r="I9" s="34"/>
       <c r="J9" s="34"/>
       <c r="K9" s="36"/>
       <c r="AT9" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AU9" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AV9" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AW9" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AX9" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AY9" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AZ9" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="BA9" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A10" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="D10" s="38" t="s">
         <v>243</v>
-      </c>
-      <c r="B10" s="30" t="s">
-        <v>84</v>
-      </c>
-      <c r="D10" s="38" t="s">
-        <v>244</v>
       </c>
       <c r="E10" s="41"/>
       <c r="F10" s="34"/>
@@ -4429,72 +4080,72 @@
       <c r="J10" s="34"/>
       <c r="K10" s="36"/>
       <c r="AT10" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AU10" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AV10" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AW10" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="AW10" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="AX10" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AY10" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AZ10" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="BA10" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:53" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="D11" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="D11" s="42" t="s">
+      <c r="E11" s="46" t="s">
         <v>79</v>
       </c>
-      <c r="E11" s="46" t="s">
+      <c r="F11" s="47" t="s">
+        <v>51</v>
+      </c>
+      <c r="G11" s="48" t="s">
         <v>80</v>
-      </c>
-      <c r="F11" s="47" t="s">
-        <v>52</v>
-      </c>
-      <c r="G11" s="48" t="s">
-        <v>81</v>
       </c>
       <c r="H11" s="42"/>
       <c r="I11" s="49" t="s">
+        <v>81</v>
+      </c>
+      <c r="J11" s="47" t="s">
+        <v>51</v>
+      </c>
+      <c r="K11" s="48" t="s">
         <v>82</v>
       </c>
-      <c r="J11" s="47" t="s">
-        <v>52</v>
-      </c>
-      <c r="K11" s="48" t="s">
-        <v>83</v>
-      </c>
       <c r="AU11" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="BA11" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:53" x14ac:dyDescent="0.2">
       <c r="AU12" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="BA12" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -4548,12 +4199,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B2" s="6"/>
     </row>
@@ -4591,12 +4242,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -4636,12 +4287,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B2" s="6"/>
     </row>
@@ -4671,12 +4322,12 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -4734,7 +4385,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
   </sheetData>
@@ -4761,12 +4412,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -4808,12 +4459,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B2" s="6"/>
     </row>
@@ -4856,12 +4507,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B2" s="6"/>
     </row>
@@ -4898,12 +4549,12 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -4947,12 +4598,12 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -4973,9 +4624,7 @@
   </sheetPr>
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4991,7 +4640,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -5061,12 +4710,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B2" s="6"/>
     </row>
@@ -5097,12 +4746,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -5135,12 +4784,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -5180,12 +4829,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -5225,12 +4874,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -5275,7 +4924,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -5307,15 +4956,15 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -5431,163 +5080,163 @@
     </row>
     <row r="2" spans="1:55" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="K2" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="L2" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="M2" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="N2" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="O2" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="P2" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="Q2" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="R2" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="S2" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="S2" s="6" t="s">
+      <c r="T2" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="T2" s="6" t="s">
+      <c r="U2" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="U2" s="6" t="s">
+      <c r="V2" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="V2" s="6" t="s">
+      <c r="W2" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="W2" s="6" t="s">
+      <c r="X2" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="X2" s="6" t="s">
+      <c r="Y2" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="Y2" s="6" t="s">
+      <c r="Z2" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="Z2" s="6" t="s">
+      <c r="AA2" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="AA2" s="6" t="s">
+      <c r="AB2" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="AB2" s="6" t="s">
+      <c r="AC2" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="AC2" s="6" t="s">
+      <c r="AD2" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="AD2" s="6" t="s">
+      <c r="AE2" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="AE2" s="6" t="s">
+      <c r="AF2" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="AF2" s="6" t="s">
+      <c r="AG2" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="AG2" s="6" t="s">
+      <c r="AH2" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="AH2" s="6" t="s">
+      <c r="AI2" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="AI2" s="6" t="s">
+      <c r="AJ2" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="AJ2" s="6" t="s">
+      <c r="AK2" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="AK2" s="6" t="s">
+      <c r="AL2" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="AL2" s="6" t="s">
+      <c r="AM2" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="AM2" s="6" t="s">
+      <c r="AN2" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="AN2" s="6" t="s">
+      <c r="AO2" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="AO2" s="6" t="s">
+      <c r="AP2" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="AP2" s="6" t="s">
+      <c r="AQ2" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="AQ2" s="6" t="s">
+      <c r="AR2" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="AR2" s="6" t="s">
+      <c r="AS2" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="AS2" s="6" t="s">
+      <c r="AT2" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="AT2" s="6" t="s">
+      <c r="AU2" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="AU2" s="6" t="s">
+      <c r="AV2" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="AV2" s="6" t="s">
+      <c r="AW2" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="AW2" s="6" t="s">
+      <c r="AX2" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="AX2" s="6" t="s">
+      <c r="AY2" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="AY2" s="6" t="s">
+      <c r="AZ2" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="AZ2" s="6" t="s">
+      <c r="BA2" s="6" t="s">
         <v>209</v>
-      </c>
-      <c r="BA2" s="6" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:55" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -5634,163 +5283,163 @@
     </row>
     <row r="2" spans="1:53" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="K2" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="L2" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="M2" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="N2" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="O2" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="P2" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="Q2" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="R2" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="S2" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="S2" s="6" t="s">
+      <c r="T2" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="T2" s="6" t="s">
+      <c r="U2" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="U2" s="6" t="s">
+      <c r="V2" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="V2" s="6" t="s">
+      <c r="W2" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="W2" s="6" t="s">
+      <c r="X2" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="X2" s="6" t="s">
+      <c r="Y2" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="Y2" s="6" t="s">
+      <c r="Z2" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="Z2" s="6" t="s">
+      <c r="AA2" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="AA2" s="6" t="s">
+      <c r="AB2" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="AB2" s="6" t="s">
+      <c r="AC2" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="AC2" s="6" t="s">
+      <c r="AD2" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="AD2" s="6" t="s">
+      <c r="AE2" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="AE2" s="6" t="s">
+      <c r="AF2" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="AF2" s="6" t="s">
+      <c r="AG2" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="AG2" s="6" t="s">
+      <c r="AH2" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="AH2" s="6" t="s">
+      <c r="AI2" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="AI2" s="6" t="s">
+      <c r="AJ2" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="AJ2" s="6" t="s">
+      <c r="AK2" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="AK2" s="6" t="s">
+      <c r="AL2" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="AL2" s="6" t="s">
+      <c r="AM2" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="AM2" s="6" t="s">
+      <c r="AN2" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="AN2" s="6" t="s">
+      <c r="AO2" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="AO2" s="6" t="s">
+      <c r="AP2" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="AP2" s="6" t="s">
+      <c r="AQ2" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="AQ2" s="6" t="s">
+      <c r="AR2" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="AR2" s="6" t="s">
+      <c r="AS2" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="AS2" s="6" t="s">
+      <c r="AT2" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="AT2" s="6" t="s">
+      <c r="AU2" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="AU2" s="6" t="s">
+      <c r="AV2" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="AV2" s="6" t="s">
+      <c r="AW2" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="AW2" s="6" t="s">
+      <c r="AX2" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="AX2" s="6" t="s">
+      <c r="AY2" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="AY2" s="6" t="s">
+      <c r="AZ2" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="AZ2" s="6" t="s">
+      <c r="BA2" s="6" t="s">
         <v>209</v>
-      </c>
-      <c r="BA2" s="6" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:53" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -6057,163 +5706,163 @@
     </row>
     <row r="2" spans="1:53" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="K2" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="L2" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="M2" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="N2" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="O2" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="P2" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="Q2" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="R2" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="S2" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="S2" s="6" t="s">
+      <c r="T2" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="T2" s="6" t="s">
+      <c r="U2" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="U2" s="6" t="s">
+      <c r="V2" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="V2" s="6" t="s">
+      <c r="W2" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="W2" s="6" t="s">
+      <c r="X2" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="X2" s="6" t="s">
+      <c r="Y2" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="Y2" s="6" t="s">
+      <c r="Z2" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="Z2" s="6" t="s">
+      <c r="AA2" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="AA2" s="6" t="s">
+      <c r="AB2" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="AB2" s="6" t="s">
+      <c r="AC2" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="AC2" s="6" t="s">
+      <c r="AD2" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="AD2" s="6" t="s">
+      <c r="AE2" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="AE2" s="6" t="s">
+      <c r="AF2" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="AF2" s="6" t="s">
+      <c r="AG2" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="AG2" s="6" t="s">
+      <c r="AH2" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="AH2" s="6" t="s">
+      <c r="AI2" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="AI2" s="6" t="s">
+      <c r="AJ2" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="AJ2" s="6" t="s">
+      <c r="AK2" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="AK2" s="6" t="s">
+      <c r="AL2" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="AL2" s="6" t="s">
+      <c r="AM2" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="AM2" s="6" t="s">
+      <c r="AN2" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="AN2" s="6" t="s">
+      <c r="AO2" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="AO2" s="6" t="s">
+      <c r="AP2" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="AP2" s="6" t="s">
+      <c r="AQ2" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="AQ2" s="6" t="s">
+      <c r="AR2" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="AR2" s="6" t="s">
+      <c r="AS2" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="AS2" s="6" t="s">
+      <c r="AT2" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="AT2" s="6" t="s">
+      <c r="AU2" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="AU2" s="6" t="s">
+      <c r="AV2" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="AV2" s="6" t="s">
+      <c r="AW2" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="AW2" s="6" t="s">
+      <c r="AX2" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="AX2" s="6" t="s">
+      <c r="AY2" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="AY2" s="6" t="s">
+      <c r="AZ2" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="AZ2" s="6" t="s">
+      <c r="BA2" s="6" t="s">
         <v>209</v>
-      </c>
-      <c r="BA2" s="6" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:53" x14ac:dyDescent="0.2">
@@ -6307,28 +5956,28 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D4" s="5"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="M5" s="6"/>
       <c r="N5" s="6"/>
@@ -6336,52 +5985,52 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -6411,16 +6060,16 @@
   <sheetData>
     <row r="1" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>247</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>248</v>
       </c>
       <c r="Q1" s="1">
         <v>0.01</v>
@@ -6428,163 +6077,163 @@
     </row>
     <row r="2" spans="1:55" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="K2" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="L2" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="M2" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="N2" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="O2" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="P2" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="Q2" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="R2" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="S2" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="S2" s="6" t="s">
+      <c r="T2" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="T2" s="6" t="s">
+      <c r="U2" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="U2" s="6" t="s">
+      <c r="V2" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="V2" s="6" t="s">
+      <c r="W2" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="W2" s="6" t="s">
+      <c r="X2" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="X2" s="6" t="s">
+      <c r="Y2" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="Y2" s="6" t="s">
+      <c r="Z2" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="Z2" s="6" t="s">
+      <c r="AA2" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="AA2" s="6" t="s">
+      <c r="AB2" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="AB2" s="6" t="s">
+      <c r="AC2" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="AC2" s="6" t="s">
+      <c r="AD2" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="AD2" s="6" t="s">
+      <c r="AE2" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="AE2" s="6" t="s">
+      <c r="AF2" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="AF2" s="6" t="s">
+      <c r="AG2" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="AG2" s="6" t="s">
+      <c r="AH2" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="AH2" s="6" t="s">
+      <c r="AI2" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="AI2" s="6" t="s">
+      <c r="AJ2" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="AJ2" s="6" t="s">
+      <c r="AK2" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="AK2" s="6" t="s">
+      <c r="AL2" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="AL2" s="6" t="s">
+      <c r="AM2" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="AM2" s="6" t="s">
+      <c r="AN2" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="AN2" s="6" t="s">
+      <c r="AO2" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="AO2" s="6" t="s">
+      <c r="AP2" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="AP2" s="6" t="s">
+      <c r="AQ2" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="AQ2" s="6" t="s">
+      <c r="AR2" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="AR2" s="6" t="s">
+      <c r="AS2" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="AS2" s="6" t="s">
+      <c r="AT2" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="AT2" s="6" t="s">
+      <c r="AU2" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="AU2" s="6" t="s">
+      <c r="AV2" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="AV2" s="6" t="s">
+      <c r="AW2" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="AW2" s="6" t="s">
+      <c r="AX2" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="AX2" s="6" t="s">
+      <c r="AY2" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="AY2" s="6" t="s">
+      <c r="AZ2" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="AZ2" s="6" t="s">
+      <c r="BA2" s="6" t="s">
         <v>209</v>
-      </c>
-      <c r="BA2" s="6" t="s">
-        <v>210</v>
       </c>
       <c r="BC2" s="1"/>
     </row>
@@ -7580,7 +7229,7 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -8117,12 +7766,12 @@
   <sheetData>
     <row r="1" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -12120,10 +11769,10 @@
     </row>
     <row r="2" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -12163,10 +11812,10 @@
     </row>
     <row r="2" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -12210,7 +11859,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -12263,163 +11912,163 @@
     </row>
     <row r="2" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="K2" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="L2" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="M2" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="N2" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="O2" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="P2" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="Q2" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="R2" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="S2" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="S2" s="6" t="s">
+      <c r="T2" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="T2" s="6" t="s">
+      <c r="U2" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="U2" s="6" t="s">
+      <c r="V2" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="V2" s="6" t="s">
+      <c r="W2" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="W2" s="6" t="s">
+      <c r="X2" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="X2" s="6" t="s">
+      <c r="Y2" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="Y2" s="6" t="s">
+      <c r="Z2" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="Z2" s="6" t="s">
+      <c r="AA2" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="AA2" s="6" t="s">
+      <c r="AB2" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="AB2" s="6" t="s">
+      <c r="AC2" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="AC2" s="6" t="s">
+      <c r="AD2" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="AD2" s="6" t="s">
+      <c r="AE2" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="AE2" s="6" t="s">
+      <c r="AF2" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="AF2" s="6" t="s">
+      <c r="AG2" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="AG2" s="6" t="s">
+      <c r="AH2" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="AH2" s="6" t="s">
+      <c r="AI2" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="AI2" s="6" t="s">
+      <c r="AJ2" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="AJ2" s="6" t="s">
+      <c r="AK2" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="AK2" s="6" t="s">
+      <c r="AL2" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="AL2" s="6" t="s">
+      <c r="AM2" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="AM2" s="6" t="s">
+      <c r="AN2" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="AN2" s="6" t="s">
+      <c r="AO2" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="AO2" s="6" t="s">
+      <c r="AP2" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="AP2" s="6" t="s">
+      <c r="AQ2" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="AQ2" s="6" t="s">
+      <c r="AR2" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="AR2" s="6" t="s">
+      <c r="AS2" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="AS2" s="6" t="s">
+      <c r="AT2" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="AT2" s="6" t="s">
+      <c r="AU2" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="AU2" s="6" t="s">
+      <c r="AV2" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="AV2" s="6" t="s">
+      <c r="AW2" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="AW2" s="6" t="s">
+      <c r="AX2" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="AX2" s="6" t="s">
+      <c r="AY2" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="AY2" s="6" t="s">
+      <c r="AZ2" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="AZ2" s="6" t="s">
+      <c r="BA2" s="6" t="s">
         <v>209</v>
-      </c>
-      <c r="BA2" s="6" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:53" x14ac:dyDescent="0.2">
@@ -12615,163 +12264,163 @@
     </row>
     <row r="2" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="K2" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="L2" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="M2" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="N2" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="O2" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="P2" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="Q2" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="R2" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="S2" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="S2" s="6" t="s">
+      <c r="T2" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="T2" s="6" t="s">
+      <c r="U2" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="U2" s="6" t="s">
+      <c r="V2" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="V2" s="6" t="s">
+      <c r="W2" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="W2" s="6" t="s">
+      <c r="X2" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="X2" s="6" t="s">
+      <c r="Y2" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="Y2" s="6" t="s">
+      <c r="Z2" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="Z2" s="6" t="s">
+      <c r="AA2" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="AA2" s="6" t="s">
+      <c r="AB2" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="AB2" s="6" t="s">
+      <c r="AC2" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="AC2" s="6" t="s">
+      <c r="AD2" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="AD2" s="6" t="s">
+      <c r="AE2" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="AE2" s="6" t="s">
+      <c r="AF2" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="AF2" s="6" t="s">
+      <c r="AG2" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="AG2" s="6" t="s">
+      <c r="AH2" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="AH2" s="6" t="s">
+      <c r="AI2" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="AI2" s="6" t="s">
+      <c r="AJ2" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="AJ2" s="6" t="s">
+      <c r="AK2" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="AK2" s="6" t="s">
+      <c r="AL2" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="AL2" s="6" t="s">
+      <c r="AM2" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="AM2" s="6" t="s">
+      <c r="AN2" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="AN2" s="6" t="s">
+      <c r="AO2" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="AO2" s="6" t="s">
+      <c r="AP2" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="AP2" s="6" t="s">
+      <c r="AQ2" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="AQ2" s="6" t="s">
+      <c r="AR2" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="AR2" s="6" t="s">
+      <c r="AS2" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="AS2" s="6" t="s">
+      <c r="AT2" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="AT2" s="6" t="s">
+      <c r="AU2" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="AU2" s="6" t="s">
+      <c r="AV2" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="AV2" s="6" t="s">
+      <c r="AW2" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="AW2" s="6" t="s">
+      <c r="AX2" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="AX2" s="6" t="s">
+      <c r="AY2" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="AY2" s="6" t="s">
+      <c r="AZ2" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="AZ2" s="6" t="s">
+      <c r="BA2" s="6" t="s">
         <v>209</v>
-      </c>
-      <c r="BA2" s="6" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:53" x14ac:dyDescent="0.2">
@@ -12965,19 +12614,19 @@
         <v>Table of Freshwater Sourcing Availability [bbl/day]</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F1" s="1">
         <v>71428.571428571406</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I1" s="1">
         <v>42857.142857142899</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="L1" s="1">
         <v>0.7</v>
@@ -12985,163 +12634,163 @@
     </row>
     <row r="2" spans="1:53" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="K2" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="L2" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="M2" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="N2" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="O2" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="P2" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="Q2" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="R2" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="S2" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="S2" s="6" t="s">
+      <c r="T2" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="T2" s="6" t="s">
+      <c r="U2" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="U2" s="6" t="s">
+      <c r="V2" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="V2" s="6" t="s">
+      <c r="W2" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="W2" s="6" t="s">
+      <c r="X2" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="X2" s="6" t="s">
+      <c r="Y2" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="Y2" s="6" t="s">
+      <c r="Z2" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="Z2" s="6" t="s">
+      <c r="AA2" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="AA2" s="6" t="s">
+      <c r="AB2" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="AB2" s="6" t="s">
+      <c r="AC2" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="AC2" s="6" t="s">
+      <c r="AD2" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="AD2" s="6" t="s">
+      <c r="AE2" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="AE2" s="6" t="s">
+      <c r="AF2" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="AF2" s="6" t="s">
+      <c r="AG2" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="AG2" s="6" t="s">
+      <c r="AH2" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="AH2" s="6" t="s">
+      <c r="AI2" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="AI2" s="6" t="s">
+      <c r="AJ2" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="AJ2" s="6" t="s">
+      <c r="AK2" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="AK2" s="6" t="s">
+      <c r="AL2" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="AL2" s="6" t="s">
+      <c r="AM2" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="AM2" s="6" t="s">
+      <c r="AN2" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="AN2" s="6" t="s">
+      <c r="AO2" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="AO2" s="6" t="s">
+      <c r="AP2" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="AP2" s="6" t="s">
+      <c r="AQ2" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="AQ2" s="6" t="s">
+      <c r="AR2" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="AR2" s="6" t="s">
+      <c r="AS2" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="AS2" s="6" t="s">
+      <c r="AT2" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="AT2" s="6" t="s">
+      <c r="AU2" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="AU2" s="6" t="s">
+      <c r="AV2" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="AV2" s="6" t="s">
+      <c r="AW2" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="AW2" s="6" t="s">
+      <c r="AX2" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="AX2" s="6" t="s">
+      <c r="AY2" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="AY2" s="6" t="s">
+      <c r="AZ2" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="AZ2" s="6" t="s">
+      <c r="BA2" s="6" t="s">
         <v>209</v>
-      </c>
-      <c r="BA2" s="6" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:53" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -13288,10 +12937,10 @@
     </row>
     <row r="2" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -13330,7 +12979,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
@@ -13375,10 +13024,10 @@
     </row>
     <row r="2" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -13415,10 +13064,10 @@
     </row>
     <row r="2" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -13492,163 +13141,163 @@
     </row>
     <row r="2" spans="1:53" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="K2" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="L2" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="M2" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="N2" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="O2" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="P2" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="Q2" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="R2" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="S2" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="S2" s="6" t="s">
+      <c r="T2" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="T2" s="6" t="s">
+      <c r="U2" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="U2" s="6" t="s">
+      <c r="V2" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="V2" s="6" t="s">
+      <c r="W2" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="W2" s="6" t="s">
+      <c r="X2" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="X2" s="6" t="s">
+      <c r="Y2" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="Y2" s="6" t="s">
+      <c r="Z2" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="Z2" s="6" t="s">
+      <c r="AA2" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="AA2" s="6" t="s">
+      <c r="AB2" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="AB2" s="6" t="s">
+      <c r="AC2" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="AC2" s="6" t="s">
+      <c r="AD2" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="AD2" s="6" t="s">
+      <c r="AE2" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="AE2" s="6" t="s">
+      <c r="AF2" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="AF2" s="6" t="s">
+      <c r="AG2" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="AG2" s="6" t="s">
+      <c r="AH2" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="AH2" s="6" t="s">
+      <c r="AI2" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="AI2" s="6" t="s">
+      <c r="AJ2" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="AJ2" s="6" t="s">
+      <c r="AK2" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="AK2" s="6" t="s">
+      <c r="AL2" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="AL2" s="6" t="s">
+      <c r="AM2" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="AM2" s="6" t="s">
+      <c r="AN2" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="AN2" s="6" t="s">
+      <c r="AO2" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="AO2" s="6" t="s">
+      <c r="AP2" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="AP2" s="6" t="s">
+      <c r="AQ2" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="AQ2" s="6" t="s">
+      <c r="AR2" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="AR2" s="6" t="s">
+      <c r="AS2" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="AS2" s="6" t="s">
+      <c r="AT2" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="AT2" s="6" t="s">
+      <c r="AU2" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="AU2" s="6" t="s">
+      <c r="AV2" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="AV2" s="6" t="s">
+      <c r="AW2" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="AW2" s="6" t="s">
+      <c r="AX2" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="AX2" s="6" t="s">
+      <c r="AY2" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="AY2" s="6" t="s">
+      <c r="AZ2" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="AZ2" s="6" t="s">
+      <c r="BA2" s="6" t="s">
         <v>209</v>
-      </c>
-      <c r="BA2" s="6" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:53" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -13662,7 +13311,7 @@
     </row>
     <row r="9" spans="1:53" x14ac:dyDescent="0.2">
       <c r="D9" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F9" s="5"/>
     </row>
@@ -13695,10 +13344,10 @@
     </row>
     <row r="2" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -13738,13 +13387,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -13826,10 +13475,10 @@
     </row>
     <row r="2" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -13865,7 +13514,7 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -14401,10 +14050,10 @@
     </row>
     <row r="2" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -14442,10 +14091,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -14499,12 +14148,12 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -14563,7 +14212,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
@@ -14613,7 +14262,7 @@
     </row>
     <row r="2" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -14664,10 +14313,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -14715,7 +14364,7 @@
     </row>
     <row r="2" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -14772,10 +14421,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -14824,10 +14473,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -14945,7 +14594,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -15025,15 +14674,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B3" s="26">
         <v>300000</v>
@@ -15070,7 +14719,7 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -15603,10 +15252,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -15663,15 +15312,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B3" s="54">
         <v>0</v>
@@ -15679,7 +15328,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B4" s="54">
         <v>14285.714285714286</v>
@@ -15687,7 +15336,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B5" s="54">
         <v>35714.285714285717</v>
@@ -15695,7 +15344,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B6" s="54">
         <v>42857.142857142855</v>
@@ -15703,7 +15352,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B7" s="54">
         <v>50000</v>
@@ -15741,7 +15390,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
@@ -15783,10 +15432,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -15835,18 +15484,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -15922,18 +15571,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -16008,15 +15657,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -16051,7 +15700,9 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -16061,15 +15712,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -16093,7 +15744,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16102,17 +15753,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="str">
-        <f>CONCATENATE( "Table with processing cost for sending water to beneficial reuse [",VLOOKUP("currency", [1]Units!$A$2:$B$11, 2, FALSE),"/", VLOOKUP("volume", [1]Units!$A$2:$B$11, 2, FALSE),"]")</f>
-        <v>Table with processing cost for sending water to beneficial reuse [USD/bbl]</v>
+      <c r="A1" s="1" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="62" t="s">
-        <v>260</v>
-      </c>
-      <c r="B2" s="62" t="s">
-        <v>46</v>
+      <c r="A2" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -16143,10 +15793,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -16183,15 +15833,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -16223,20 +15873,20 @@
   <sheetData>
     <row r="1" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B3" s="25">
         <v>110</v>
@@ -16244,7 +15894,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="21" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B4" s="30">
         <v>0.03</v>
@@ -16252,24 +15902,24 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="21" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B5" s="25">
         <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B6" s="26">
         <v>150</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -16296,20 +15946,20 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B3" s="30">
         <v>0.08</v>
@@ -16317,7 +15967,7 @@
     </row>
     <row r="4" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B4" s="26">
         <v>20</v>
@@ -16354,7 +16004,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
@@ -16405,10 +16055,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -16461,10 +16111,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -16510,10 +16160,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -16555,10 +16205,10 @@
     </row>
     <row r="2" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -16679,7 +16329,7 @@
     </row>
     <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -16723,7 +16373,7 @@
     </row>
     <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -16778,15 +16428,15 @@
     </row>
     <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B3" s="57">
         <v>0.2</v>
@@ -16819,10 +16469,10 @@
     </row>
     <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>

</xml_diff>

<commit_message>
add disposal tabs to template, parser
</commit_message>
<xml_diff>
--- a/backend/app/internal/assets/pareto_input_template.xlsx
+++ b/backend/app/internal/assets/pareto_input_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelpesce/Desktop/pareto-ui/backend/app/internal/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A35B2066-22E2-6947-9679-4DF36C426259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{674FCFAE-6040-9643-A197-CF9F86586D27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35000" yWindow="500" windowWidth="34560" windowHeight="18980" tabRatio="953" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="0" yWindow="8440" windowWidth="34560" windowHeight="11780" tabRatio="953" firstSheet="94" activeTab="102" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -110,6 +110,13 @@
     <sheet name="StorageExpansionLeadTime" sheetId="130" r:id="rId95"/>
     <sheet name="PipelineExpansionLeadTime_Dist" sheetId="131" r:id="rId96"/>
     <sheet name="PipelineExpansionLeadTime_Capac" sheetId="132" r:id="rId97"/>
+    <sheet name="SWDDeep" sheetId="137" r:id="rId98"/>
+    <sheet name="SWDAveragePressure" sheetId="138" r:id="rId99"/>
+    <sheet name="SWDProxPAWell" sheetId="139" r:id="rId100"/>
+    <sheet name="SWDProxInactiveWell" sheetId="140" r:id="rId101"/>
+    <sheet name="SWDProxEQ" sheetId="141" r:id="rId102"/>
+    <sheet name="SWDProxFault" sheetId="142" r:id="rId103"/>
+    <sheet name="SWDProxHpOrLpWell" sheetId="143" r:id="rId104"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="76" hidden="1">#REF!</definedName>
@@ -137,7 +144,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="273">
   <si>
     <t>Data Input Spreadsheet Overview</t>
   </si>
@@ -935,6 +942,27 @@
   </si>
   <si>
     <t>Table with processing cost for sending water to beneficial reuse [USD/bbl]</t>
+  </si>
+  <si>
+    <t>SWDs - shallow (0) or deep (1)</t>
+  </si>
+  <si>
+    <t>Average pressure/depth in vicinity of well [psi/ft]</t>
+  </si>
+  <si>
+    <t>Table of SWD proximity to P&amp;A'd well [miles]</t>
+  </si>
+  <si>
+    <t>Table of SWD proximity to inactive/temporarily abandoned formerly producing well (completed prior to 2000) [miles]</t>
+  </si>
+  <si>
+    <t>Table of SWD proximity to earthquakes &gt;= 3.0 magnitude [miles]</t>
+  </si>
+  <si>
+    <t>Table of SWD proximity to high pressure or low pressure injection well [miles]</t>
+  </si>
+  <si>
+    <t>Table of SWD proximity to fault [miles]</t>
   </si>
 </sst>
 </file>
@@ -1316,7 +1344,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1447,6 +1475,9 @@
     <xf numFmtId="3" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -1474,9 +1505,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1514,7 +1545,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1620,7 +1651,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1762,7 +1793,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1775,7 +1806,7 @@
   </sheetPr>
   <dimension ref="B1:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2379,6 +2410,151 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet100.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43624E75-14B8-7140-AAB7-78C62C7F81B5}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B2" s="62" t="s">
+        <v>220</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet101.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F7A3D56-D0E0-7644-9ABD-B2C2305B3F6F}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B2" s="62" t="s">
+        <v>220</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet102.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B595BF9D-C714-6543-BB99-6BB0195667C1}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B2" s="62" t="s">
+        <v>220</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet103.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6476C4B-E64B-424F-922F-3419F696DC11}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B2" s="62" t="s">
+        <v>220</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet104.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71CE3F0B-DA65-4644-89E8-69C54E8A2D09}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B2" s="62" t="s">
+        <v>220</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -16509,4 +16685,62 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet98.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6386754-0298-0143-B5D2-5311F4AFDC4F}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B2" s="62" t="s">
+        <v>220</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet99.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8B0FD37-6B38-5E47-A627-F3BDABA7E934}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B2" s="62" t="s">
+        <v>220</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add additional missing tabs to input template
</commit_message>
<xml_diff>
--- a/backend/app/internal/assets/pareto_input_template.xlsx
+++ b/backend/app/internal/assets/pareto_input_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelpesce/Desktop/pareto-ui/backend/app/internal/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{674FCFAE-6040-9643-A197-CF9F86586D27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67504026-352D-3B42-A427-3C635667645F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="8440" windowWidth="34560" windowHeight="11780" tabRatio="953" firstSheet="94" activeTab="102" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="0" yWindow="8440" windowWidth="34560" windowHeight="11780" tabRatio="953" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -105,19 +105,25 @@
     <sheet name="PadWaterQuality" sheetId="99" r:id="rId90"/>
     <sheet name="StorageInitialWaterQuality" sheetId="100" r:id="rId91"/>
     <sheet name="PadStorageInitialWaterQuality" sheetId="101" r:id="rId92"/>
-    <sheet name="TreatmentExpansionLeadTime" sheetId="128" r:id="rId93"/>
-    <sheet name="DisposalExpansionLeadTime" sheetId="129" r:id="rId94"/>
-    <sheet name="StorageExpansionLeadTime" sheetId="130" r:id="rId95"/>
-    <sheet name="PipelineExpansionLeadTime_Dist" sheetId="131" r:id="rId96"/>
-    <sheet name="PipelineExpansionLeadTime_Capac" sheetId="132" r:id="rId97"/>
-    <sheet name="SWDDeep" sheetId="137" r:id="rId98"/>
-    <sheet name="SWDAveragePressure" sheetId="138" r:id="rId99"/>
-    <sheet name="SWDProxPAWell" sheetId="139" r:id="rId100"/>
-    <sheet name="SWDProxInactiveWell" sheetId="140" r:id="rId101"/>
-    <sheet name="SWDProxEQ" sheetId="141" r:id="rId102"/>
-    <sheet name="SWDProxFault" sheetId="142" r:id="rId103"/>
-    <sheet name="SWDProxHpOrLpWell" sheetId="143" r:id="rId104"/>
+    <sheet name="AirEmissionCoefficients" sheetId="145" r:id="rId93"/>
+    <sheet name="TreatmentEmissionCoefficients" sheetId="144" r:id="rId94"/>
+    <sheet name="TreatmentExpansionLeadTime" sheetId="128" r:id="rId95"/>
+    <sheet name="DisposalExpansionLeadTime" sheetId="129" r:id="rId96"/>
+    <sheet name="StorageExpansionLeadTime" sheetId="130" r:id="rId97"/>
+    <sheet name="PipelineExpansionLeadTime_Dist" sheetId="131" r:id="rId98"/>
+    <sheet name="PipelineExpansionLeadTime_Capac" sheetId="132" r:id="rId99"/>
+    <sheet name="SWDDeep" sheetId="137" r:id="rId100"/>
+    <sheet name="SWDAveragePressure" sheetId="138" r:id="rId101"/>
+    <sheet name="SWDProxPAWell" sheetId="139" r:id="rId102"/>
+    <sheet name="SWDProxInactiveWell" sheetId="140" r:id="rId103"/>
+    <sheet name="SWDProxEQ" sheetId="141" r:id="rId104"/>
+    <sheet name="SWDProxFault" sheetId="142" r:id="rId105"/>
+    <sheet name="SWDProxHpOrLpWell" sheetId="143" r:id="rId106"/>
+    <sheet name="SWDRiskFactors" sheetId="146" r:id="rId107"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId108"/>
+  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="76" hidden="1">#REF!</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">TreatmentTechnologies!$A$1:$A$5</definedName>
@@ -144,7 +150,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="293">
   <si>
     <t>Data Input Spreadsheet Overview</t>
   </si>
@@ -963,6 +969,66 @@
   </si>
   <si>
     <t>Table of SWD proximity to fault [miles]</t>
+  </si>
+  <si>
+    <t>CO2</t>
+  </si>
+  <si>
+    <t>NH3</t>
+  </si>
+  <si>
+    <t>NOx</t>
+  </si>
+  <si>
+    <t>SO2</t>
+  </si>
+  <si>
+    <t>PM 2.5</t>
+  </si>
+  <si>
+    <t>OARO</t>
+  </si>
+  <si>
+    <t>SWD risk factors</t>
+  </si>
+  <si>
+    <t>orphan_well_distance_risk_factor</t>
+  </si>
+  <si>
+    <t>orphan_well_severity_risk_factor</t>
+  </si>
+  <si>
+    <t>inactive_well_distance_risk_factor</t>
+  </si>
+  <si>
+    <t>inactive_well_severity_risk_factor</t>
+  </si>
+  <si>
+    <t>EQ_distance_risk_factor</t>
+  </si>
+  <si>
+    <t>EQ_severity_risk_factor</t>
+  </si>
+  <si>
+    <t>fault_distance_risk_factor</t>
+  </si>
+  <si>
+    <t>fault_severity_risk_factor</t>
+  </si>
+  <si>
+    <t>HP_LP_distance_risk_factor</t>
+  </si>
+  <si>
+    <t>HP_LP_severity_risk_factor</t>
+  </si>
+  <si>
+    <t>HP_threshold</t>
+  </si>
+  <si>
+    <t>psi/ft</t>
+  </si>
+  <si>
+    <t>LP_threshold</t>
   </si>
 </sst>
 </file>
@@ -1073,7 +1139,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -1338,13 +1404,104 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1478,6 +1635,58 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -1502,6 +1711,329 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Overview"/>
+      <sheetName val="Schematic"/>
+      <sheetName val="Units"/>
+      <sheetName val="ProductionPads"/>
+      <sheetName val="ProductionTanks"/>
+      <sheetName val="CompletionsPads"/>
+      <sheetName val="SWDSites"/>
+      <sheetName val="ExternalWaterSources"/>
+      <sheetName val="WaterQualityComponents"/>
+      <sheetName val="AirEmissionsComponents"/>
+      <sheetName val="StorageSites"/>
+      <sheetName val="TreatmentSites"/>
+      <sheetName val="TreatmentTechnologies"/>
+      <sheetName val="ReuseOptions"/>
+      <sheetName val="NetworkNodes"/>
+      <sheetName val="PipelineDiameters"/>
+      <sheetName val="StorageCapacities"/>
+      <sheetName val="TreatmentCapacities"/>
+      <sheetName val="InjectionCapacities"/>
+      <sheetName val="PNA"/>
+      <sheetName val="CNA"/>
+      <sheetName val="CCA"/>
+      <sheetName val="NNA"/>
+      <sheetName val="NCA"/>
+      <sheetName val="NKA"/>
+      <sheetName val="NRA"/>
+      <sheetName val="NSA"/>
+      <sheetName val="NOA"/>
+      <sheetName val="SNA"/>
+      <sheetName val="SOA"/>
+      <sheetName val="FCA"/>
+      <sheetName val="RCA"/>
+      <sheetName val="RSA"/>
+      <sheetName val="SCA"/>
+      <sheetName val="RNA"/>
+      <sheetName val="ROA"/>
+      <sheetName val="RKA"/>
+      <sheetName val="PCT"/>
+      <sheetName val="FCT"/>
+      <sheetName val="PKT"/>
+      <sheetName val="CKT"/>
+      <sheetName val="CCT"/>
+      <sheetName val="CST"/>
+      <sheetName val="RST"/>
+      <sheetName val="ROT"/>
+      <sheetName val="SOT"/>
+      <sheetName val="RKT"/>
+      <sheetName val="Elevation"/>
+      <sheetName val="CompletionsDemand"/>
+      <sheetName val="PadRates"/>
+      <sheetName val="FlowbackRates"/>
+      <sheetName val="WellPressure"/>
+      <sheetName val="InitialPipelineCapacity"/>
+      <sheetName val="InitialPipelineDiameters"/>
+      <sheetName val="InitialDisposalCapacity"/>
+      <sheetName val="InitialStorageCapacity"/>
+      <sheetName val="InitialTreatmentCapacity"/>
+      <sheetName val="ReuseMinimum"/>
+      <sheetName val="ReuseCapacity"/>
+      <sheetName val="ExtWaterSourcingAvailability"/>
+      <sheetName val="CompletionsPadStorage"/>
+      <sheetName val="PadOffloadingCapacity"/>
+      <sheetName val="NodeCapacities"/>
+      <sheetName val="DisposalOperatingCapacity"/>
+      <sheetName val="DisposalOperationalCost"/>
+      <sheetName val="TreatmentOperationalCost"/>
+      <sheetName val="ReuseOperationalCost"/>
+      <sheetName val="PipelineOperationalCost"/>
+      <sheetName val="ExternalSourcingCost"/>
+      <sheetName val="TruckingHourlyCost"/>
+      <sheetName val="TruckingTime"/>
+      <sheetName val="DisposalExpansionCost"/>
+      <sheetName val="DisposalCapacityIncrements"/>
+      <sheetName val="StorageExpansionCost"/>
+      <sheetName val="StorageCapacityIncrements"/>
+      <sheetName val="TreatmentExpansionCost"/>
+      <sheetName val="TreatmentCapacityIncrements"/>
+      <sheetName val="PipelineCapexDistanceBased"/>
+      <sheetName val="PipelineExpansionDistance"/>
+      <sheetName val="PipelineCapexCapacityBased"/>
+      <sheetName val="PipelineCapacityIncrements"/>
+      <sheetName val="PipelineDiameterValues"/>
+      <sheetName val="TreatmentEfficiency"/>
+      <sheetName val="RemovalEfficiency"/>
+      <sheetName val="DesalinationTechnologies"/>
+      <sheetName val="DesalinationSites"/>
+      <sheetName val="BeneficialReuseCost"/>
+      <sheetName val="BeneficialReuseCredit"/>
+      <sheetName val="CompletionsPadOutsideSystem"/>
+      <sheetName val="Hydraulics"/>
+      <sheetName val="Economics"/>
+      <sheetName val="ExternalWaterQuality"/>
+      <sheetName val="PadWaterQuality"/>
+      <sheetName val="StorageInitialWaterQuality"/>
+      <sheetName val="AirEmissionCoefficients"/>
+      <sheetName val="TreatmentEmissionCoefficients"/>
+      <sheetName val="PadStorageInitialWaterQuality"/>
+      <sheetName val="TreatmentExpansionLeadTime"/>
+      <sheetName val="DisposalExpansionLeadTime"/>
+      <sheetName val="StorageExpansionLeadTime"/>
+      <sheetName val="PipelineExpansionLeadTime_Dist"/>
+      <sheetName val="PipelineExpansionLeadTime_Capac"/>
+      <sheetName val="SWDDeep"/>
+      <sheetName val="SWDAveragePressure"/>
+      <sheetName val="SWDProxPAWell"/>
+      <sheetName val="SWDProxInactiveWell"/>
+      <sheetName val="SWDProxEQ"/>
+      <sheetName val="SWDProxFault"/>
+      <sheetName val="SWDProxHpOrLpWell"/>
+      <sheetName val="SWDRiskFactors"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2">
+        <row r="2">
+          <cell r="A2" t="str">
+            <v>INDEX</v>
+          </cell>
+          <cell r="B2" t="str">
+            <v>VALUE</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v>volume</v>
+          </cell>
+          <cell r="B3" t="str">
+            <v>bbl</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4" t="str">
+            <v>distance</v>
+          </cell>
+          <cell r="B4" t="str">
+            <v>mile</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5" t="str">
+            <v>diameter</v>
+          </cell>
+          <cell r="B5" t="str">
+            <v>inch</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6" t="str">
+            <v>concentration</v>
+          </cell>
+          <cell r="B6" t="str">
+            <v>mg/liter</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7" t="str">
+            <v>currency</v>
+          </cell>
+          <cell r="B7" t="str">
+            <v>USD</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8" t="str">
+            <v>time</v>
+          </cell>
+          <cell r="B8" t="str">
+            <v>day</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9" t="str">
+            <v>pressure</v>
+          </cell>
+          <cell r="B9" t="str">
+            <v>psi</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10" t="str">
+            <v>elevation</v>
+          </cell>
+          <cell r="B10" t="str">
+            <v>foot</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11" t="str">
+            <v>decision period</v>
+          </cell>
+          <cell r="B11" t="str">
+            <v>week</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12" t="str">
+            <v>mass</v>
+          </cell>
+          <cell r="B12" t="str">
+            <v>g</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
+      <sheetData sheetId="26"/>
+      <sheetData sheetId="27"/>
+      <sheetData sheetId="28"/>
+      <sheetData sheetId="29"/>
+      <sheetData sheetId="30"/>
+      <sheetData sheetId="31"/>
+      <sheetData sheetId="32"/>
+      <sheetData sheetId="33"/>
+      <sheetData sheetId="34"/>
+      <sheetData sheetId="35"/>
+      <sheetData sheetId="36"/>
+      <sheetData sheetId="37"/>
+      <sheetData sheetId="38"/>
+      <sheetData sheetId="39"/>
+      <sheetData sheetId="40"/>
+      <sheetData sheetId="41"/>
+      <sheetData sheetId="42"/>
+      <sheetData sheetId="43"/>
+      <sheetData sheetId="44"/>
+      <sheetData sheetId="45"/>
+      <sheetData sheetId="46"/>
+      <sheetData sheetId="47"/>
+      <sheetData sheetId="48"/>
+      <sheetData sheetId="49"/>
+      <sheetData sheetId="50"/>
+      <sheetData sheetId="51"/>
+      <sheetData sheetId="52"/>
+      <sheetData sheetId="53"/>
+      <sheetData sheetId="54"/>
+      <sheetData sheetId="55"/>
+      <sheetData sheetId="56"/>
+      <sheetData sheetId="57"/>
+      <sheetData sheetId="58"/>
+      <sheetData sheetId="59"/>
+      <sheetData sheetId="60"/>
+      <sheetData sheetId="61"/>
+      <sheetData sheetId="62"/>
+      <sheetData sheetId="63"/>
+      <sheetData sheetId="64"/>
+      <sheetData sheetId="65"/>
+      <sheetData sheetId="66"/>
+      <sheetData sheetId="67"/>
+      <sheetData sheetId="68"/>
+      <sheetData sheetId="69"/>
+      <sheetData sheetId="70"/>
+      <sheetData sheetId="71"/>
+      <sheetData sheetId="72"/>
+      <sheetData sheetId="73"/>
+      <sheetData sheetId="74"/>
+      <sheetData sheetId="75"/>
+      <sheetData sheetId="76"/>
+      <sheetData sheetId="77"/>
+      <sheetData sheetId="78"/>
+      <sheetData sheetId="79"/>
+      <sheetData sheetId="80"/>
+      <sheetData sheetId="81"/>
+      <sheetData sheetId="82"/>
+      <sheetData sheetId="83"/>
+      <sheetData sheetId="84"/>
+      <sheetData sheetId="85"/>
+      <sheetData sheetId="86"/>
+      <sheetData sheetId="87"/>
+      <sheetData sheetId="88"/>
+      <sheetData sheetId="89"/>
+      <sheetData sheetId="90"/>
+      <sheetData sheetId="91"/>
+      <sheetData sheetId="92"/>
+      <sheetData sheetId="93"/>
+      <sheetData sheetId="94"/>
+      <sheetData sheetId="95"/>
+      <sheetData sheetId="96"/>
+      <sheetData sheetId="97"/>
+      <sheetData sheetId="98"/>
+      <sheetData sheetId="99"/>
+      <sheetData sheetId="100"/>
+      <sheetData sheetId="101"/>
+      <sheetData sheetId="102"/>
+      <sheetData sheetId="103"/>
+      <sheetData sheetId="104"/>
+      <sheetData sheetId="105"/>
+      <sheetData sheetId="106"/>
+      <sheetData sheetId="107"/>
+      <sheetData sheetId="108"/>
+      <sheetData sheetId="109"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1806,7 +2338,7 @@
   </sheetPr>
   <dimension ref="B1:M37"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2414,6 +2946,64 @@
 </file>
 
 <file path=xl/worksheets/sheet100.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6386754-0298-0143-B5D2-5311F4AFDC4F}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B2" s="62" t="s">
+        <v>220</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet101.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8B0FD37-6B38-5E47-A627-F3BDABA7E934}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B2" s="62" t="s">
+        <v>220</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet102.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43624E75-14B8-7140-AAB7-78C62C7F81B5}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -2442,7 +3032,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet101.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet103.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F7A3D56-D0E0-7644-9ABD-B2C2305B3F6F}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -2471,7 +3061,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet102.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet104.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B595BF9D-C714-6543-BB99-6BB0195667C1}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -2500,11 +3090,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet103.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet105.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6476C4B-E64B-424F-922F-3419F696DC11}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
@@ -2529,7 +3119,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet104.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet106.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71CE3F0B-DA65-4644-89E8-69C54E8A2D09}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -2551,6 +3141,143 @@
       </c>
       <c r="B2" s="62" t="s">
         <v>220</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet107.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B272D204-9BC5-9F40-90B0-3D3E0DFE6A2D}">
+  <sheetPr>
+    <tabColor theme="1" tint="0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="33.83203125" style="74" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.1640625" style="74"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="73" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="75" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="76" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="77" t="s">
+        <v>280</v>
+      </c>
+      <c r="B3" s="78">
+        <v>1.86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="77" t="s">
+        <v>281</v>
+      </c>
+      <c r="B4" s="78">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="77" t="s">
+        <v>282</v>
+      </c>
+      <c r="B5" s="78">
+        <v>1.86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="77" t="s">
+        <v>283</v>
+      </c>
+      <c r="B6" s="78">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="77" t="s">
+        <v>284</v>
+      </c>
+      <c r="B7" s="78">
+        <v>5.59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="77" t="s">
+        <v>285</v>
+      </c>
+      <c r="B8" s="78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="77" t="s">
+        <v>286</v>
+      </c>
+      <c r="B9" s="78">
+        <v>5.59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="77" t="s">
+        <v>287</v>
+      </c>
+      <c r="B10" s="78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="77" t="s">
+        <v>288</v>
+      </c>
+      <c r="B11" s="78">
+        <v>1.86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="77" t="s">
+        <v>289</v>
+      </c>
+      <c r="B12" s="78">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="77" t="s">
+        <v>290</v>
+      </c>
+      <c r="B13" s="78">
+        <v>0.7</v>
+      </c>
+      <c r="C13" s="74" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="79" t="s">
+        <v>292</v>
+      </c>
+      <c r="B14" s="80">
+        <v>0.5</v>
+      </c>
+      <c r="C14" s="74" t="s">
+        <v>291</v>
       </c>
     </row>
   </sheetData>
@@ -16352,6 +17079,315 @@
 </file>
 
 <file path=xl/worksheets/sheet93.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73C69F2D-49DC-1944-BFFB-2EEA9F71D13F}">
+  <sheetPr>
+    <tabColor theme="8" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="62.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT( "Table of Air Emissions Coefficients ")</f>
+        <v xml:space="preserve">Table of Air Emissions Coefficients </v>
+      </c>
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="72" t="s">
+        <v>273</v>
+      </c>
+      <c r="C2" s="64" t="s">
+        <v>274</v>
+      </c>
+      <c r="D2" s="64" t="s">
+        <v>275</v>
+      </c>
+      <c r="E2" s="64" t="s">
+        <v>276</v>
+      </c>
+      <c r="F2" s="65" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="21" t="str">
+        <f>_xlfn.CONCAT("Trucking [", VLOOKUP("mass", [1]Units!A2:B12, 2, FALSE), "/hour]")</f>
+        <v>Trucking [g/hour]</v>
+      </c>
+      <c r="B3" s="67">
+        <v>2035000</v>
+      </c>
+      <c r="C3" s="67">
+        <v>35.75</v>
+      </c>
+      <c r="D3" s="67">
+        <v>12649.999999999998</v>
+      </c>
+      <c r="E3" s="67">
+        <v>770.00000000000011</v>
+      </c>
+      <c r="F3" s="68">
+        <v>120.99999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="21" t="str">
+        <f>_xlfn.CONCAT("Pipeline Operations [", VLOOKUP("mass", [1]Units!A2:B12, 2, FALSE), "/(", VLOOKUP("volume", [1]Units!A2:B12, 2, FALSE), "*", VLOOKUP("distance", [1]Units!A2:B12, 2, FALSE), ")]")</f>
+        <v>Pipeline Operations [g/(bbl*mile)]</v>
+      </c>
+      <c r="B4" s="67">
+        <v>22</v>
+      </c>
+      <c r="C4" s="67">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="D4" s="67">
+        <v>1.4E-2</v>
+      </c>
+      <c r="E4" s="67">
+        <v>7.1000000000000004E-3</v>
+      </c>
+      <c r="F4" s="68">
+        <v>8.5999999999999998E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="21" t="str">
+        <f>_xlfn.CONCAT("Pipeline Installation [", VLOOKUP("mass", [1]Units!A2:B12, 2, FALSE), "/", VLOOKUP("distance", [1]Units!A2:B12, 2, FALSE), "]")</f>
+        <v>Pipeline Installation [g/mile]</v>
+      </c>
+      <c r="B5" s="67">
+        <v>310000000</v>
+      </c>
+      <c r="C5" s="67">
+        <v>2800</v>
+      </c>
+      <c r="D5" s="67">
+        <v>190000</v>
+      </c>
+      <c r="E5" s="67">
+        <v>100000</v>
+      </c>
+      <c r="F5" s="68">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="21" t="str">
+        <f>_xlfn.CONCAT("Disposal [", VLOOKUP("mass", [1]Units!A2:B12, 2, FALSE), "/", VLOOKUP("volume", [1]Units!A2:B12, 2, FALSE), "]")</f>
+        <v>Disposal [g/bbl]</v>
+      </c>
+      <c r="B6" s="67">
+        <v>970</v>
+      </c>
+      <c r="C6" s="67">
+        <v>0.13</v>
+      </c>
+      <c r="D6" s="67">
+        <v>9.5</v>
+      </c>
+      <c r="E6" s="67">
+        <v>2.8</v>
+      </c>
+      <c r="F6" s="68">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="str">
+        <f>_xlfn.CONCAT("Storage [", VLOOKUP("mass", [1]Units!A2:B12, 2, FALSE), "/(", VLOOKUP("volume", [1]Units!A2:B12, 2, FALSE), "*", VLOOKUP("decision period", [1]Units!A2:B12, 2, FALSE), ")]")</f>
+        <v>Storage [g/(bbl*week)]</v>
+      </c>
+      <c r="B7" s="70">
+        <v>1000</v>
+      </c>
+      <c r="C7" s="70">
+        <v>1.2E-2</v>
+      </c>
+      <c r="D7" s="70">
+        <v>2</v>
+      </c>
+      <c r="E7" s="70">
+        <v>0.65</v>
+      </c>
+      <c r="F7" s="71">
+        <v>7.5999999999999998E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet94.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE0936AA-9CB5-FA48-AA26-19FC94AF5C3A}">
+  <sheetPr>
+    <tabColor theme="8" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="str">
+        <f>_xlfn.CONCAT("Table of Air Emissions Coefficients for Treatment Technologies [", VLOOKUP("mass", [1]Units!A2:B12, 2, FALSE), "/", VLOOKUP("volume", [1]Units!A2:B12, 2, FALSE), "]")</f>
+        <v>Table of Air Emissions Coefficients for Treatment Technologies [g/bbl]</v>
+      </c>
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="63" t="s">
+        <v>213</v>
+      </c>
+      <c r="B2" s="64" t="s">
+        <v>273</v>
+      </c>
+      <c r="C2" s="64" t="s">
+        <v>274</v>
+      </c>
+      <c r="D2" s="64" t="s">
+        <v>275</v>
+      </c>
+      <c r="E2" s="64" t="s">
+        <v>276</v>
+      </c>
+      <c r="F2" s="65" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="66" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" s="67">
+        <v>9600</v>
+      </c>
+      <c r="C3" s="67">
+        <v>1.45</v>
+      </c>
+      <c r="D3" s="67">
+        <v>12.8</v>
+      </c>
+      <c r="E3" s="67">
+        <v>13.5</v>
+      </c>
+      <c r="F3" s="68">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="66" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4" s="67">
+        <v>9600</v>
+      </c>
+      <c r="C4" s="67">
+        <v>1.45</v>
+      </c>
+      <c r="D4" s="67">
+        <v>12.8</v>
+      </c>
+      <c r="E4" s="67">
+        <v>13.5</v>
+      </c>
+      <c r="F4" s="68">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="66" t="s">
+        <v>234</v>
+      </c>
+      <c r="B5" s="67">
+        <v>9600</v>
+      </c>
+      <c r="C5" s="67">
+        <v>1.45</v>
+      </c>
+      <c r="D5" s="67">
+        <v>12.8</v>
+      </c>
+      <c r="E5" s="67">
+        <v>13.5</v>
+      </c>
+      <c r="F5" s="68">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="66" t="s">
+        <v>235</v>
+      </c>
+      <c r="B6" s="67">
+        <v>9600</v>
+      </c>
+      <c r="C6" s="67">
+        <v>1.45</v>
+      </c>
+      <c r="D6" s="67">
+        <v>12.8</v>
+      </c>
+      <c r="E6" s="67">
+        <v>13.5</v>
+      </c>
+      <c r="F6" s="68">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="69" t="s">
+        <v>278</v>
+      </c>
+      <c r="B7" s="70">
+        <v>9600</v>
+      </c>
+      <c r="C7" s="70">
+        <v>1.45</v>
+      </c>
+      <c r="D7" s="70">
+        <v>12.8</v>
+      </c>
+      <c r="E7" s="70">
+        <v>13.5</v>
+      </c>
+      <c r="F7" s="71">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet95.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B28A4AC-774D-4F01-8B4F-3E23D6A50C57}">
   <sheetPr>
     <tabColor theme="0"/>
@@ -16481,7 +17517,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet94.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet96.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7A3376C-B8BF-456A-9F8F-97FD96566A3A}">
   <sheetPr>
     <tabColor theme="0"/>
@@ -16525,7 +17561,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet95.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet97.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF7EC6F2-1522-42F6-A09A-9709AB96F608}">
   <sheetPr>
     <tabColor theme="0"/>
@@ -16582,7 +17618,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet96.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet98.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F03D31AA-46D4-464A-9A51-F7F7B8767B7B}">
   <sheetPr>
     <tabColor theme="0"/>
@@ -16623,7 +17659,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet97.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet99.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3C876A9-1E8F-4C0D-BF38-C23F08A2F8DA}">
   <sheetPr>
     <tabColor theme="0"/>
@@ -16685,62 +17721,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet98.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6386754-0298-0143-B5D2-5311F4AFDC4F}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="B1" s="1"/>
-    </row>
-    <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="B2" s="62" t="s">
-        <v>220</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet99.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8B0FD37-6B38-5E47-A627-F3BDABA7E934}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="B1" s="1"/>
-    </row>
-    <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="B2" s="62" t="s">
-        <v>220</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
update template - remove links (these are local and were breaking things)
</commit_message>
<xml_diff>
--- a/backend/app/internal/assets/pareto_input_template.xlsx
+++ b/backend/app/internal/assets/pareto_input_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelpesce/Desktop/pareto-ui/backend/app/internal/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67504026-352D-3B42-A427-3C635667645F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB01BD66-9588-CB48-B64D-3976CAFC7CDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="8440" windowWidth="34560" windowHeight="11780" tabRatio="953" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="0" yWindow="1360" windowWidth="34560" windowHeight="18300" tabRatio="953" firstSheet="86" activeTab="93" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -121,9 +121,6 @@
     <sheet name="SWDProxHpOrLpWell" sheetId="143" r:id="rId106"/>
     <sheet name="SWDRiskFactors" sheetId="146" r:id="rId107"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId108"/>
-  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="76" hidden="1">#REF!</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">TreatmentTechnologies!$A$1:$A$5</definedName>
@@ -150,7 +147,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="299">
   <si>
     <t>Data Input Spreadsheet Overview</t>
   </si>
@@ -1029,6 +1026,24 @@
   </si>
   <si>
     <t>LP_threshold</t>
+  </si>
+  <si>
+    <t>Trucking [g/hour]</t>
+  </si>
+  <si>
+    <t>Pipeline Operations [g/(bbl*mile)]</t>
+  </si>
+  <si>
+    <t>Pipeline Installation [g/mile]</t>
+  </si>
+  <si>
+    <t>Disposal [g/bbl]</t>
+  </si>
+  <si>
+    <t>Storage [g/(bbl*week)]</t>
+  </si>
+  <si>
+    <t>Table of Air Emissions Coefficients for Treatment Technologies [g/bbl]</t>
   </si>
 </sst>
 </file>
@@ -1713,329 +1728,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Overview"/>
-      <sheetName val="Schematic"/>
-      <sheetName val="Units"/>
-      <sheetName val="ProductionPads"/>
-      <sheetName val="ProductionTanks"/>
-      <sheetName val="CompletionsPads"/>
-      <sheetName val="SWDSites"/>
-      <sheetName val="ExternalWaterSources"/>
-      <sheetName val="WaterQualityComponents"/>
-      <sheetName val="AirEmissionsComponents"/>
-      <sheetName val="StorageSites"/>
-      <sheetName val="TreatmentSites"/>
-      <sheetName val="TreatmentTechnologies"/>
-      <sheetName val="ReuseOptions"/>
-      <sheetName val="NetworkNodes"/>
-      <sheetName val="PipelineDiameters"/>
-      <sheetName val="StorageCapacities"/>
-      <sheetName val="TreatmentCapacities"/>
-      <sheetName val="InjectionCapacities"/>
-      <sheetName val="PNA"/>
-      <sheetName val="CNA"/>
-      <sheetName val="CCA"/>
-      <sheetName val="NNA"/>
-      <sheetName val="NCA"/>
-      <sheetName val="NKA"/>
-      <sheetName val="NRA"/>
-      <sheetName val="NSA"/>
-      <sheetName val="NOA"/>
-      <sheetName val="SNA"/>
-      <sheetName val="SOA"/>
-      <sheetName val="FCA"/>
-      <sheetName val="RCA"/>
-      <sheetName val="RSA"/>
-      <sheetName val="SCA"/>
-      <sheetName val="RNA"/>
-      <sheetName val="ROA"/>
-      <sheetName val="RKA"/>
-      <sheetName val="PCT"/>
-      <sheetName val="FCT"/>
-      <sheetName val="PKT"/>
-      <sheetName val="CKT"/>
-      <sheetName val="CCT"/>
-      <sheetName val="CST"/>
-      <sheetName val="RST"/>
-      <sheetName val="ROT"/>
-      <sheetName val="SOT"/>
-      <sheetName val="RKT"/>
-      <sheetName val="Elevation"/>
-      <sheetName val="CompletionsDemand"/>
-      <sheetName val="PadRates"/>
-      <sheetName val="FlowbackRates"/>
-      <sheetName val="WellPressure"/>
-      <sheetName val="InitialPipelineCapacity"/>
-      <sheetName val="InitialPipelineDiameters"/>
-      <sheetName val="InitialDisposalCapacity"/>
-      <sheetName val="InitialStorageCapacity"/>
-      <sheetName val="InitialTreatmentCapacity"/>
-      <sheetName val="ReuseMinimum"/>
-      <sheetName val="ReuseCapacity"/>
-      <sheetName val="ExtWaterSourcingAvailability"/>
-      <sheetName val="CompletionsPadStorage"/>
-      <sheetName val="PadOffloadingCapacity"/>
-      <sheetName val="NodeCapacities"/>
-      <sheetName val="DisposalOperatingCapacity"/>
-      <sheetName val="DisposalOperationalCost"/>
-      <sheetName val="TreatmentOperationalCost"/>
-      <sheetName val="ReuseOperationalCost"/>
-      <sheetName val="PipelineOperationalCost"/>
-      <sheetName val="ExternalSourcingCost"/>
-      <sheetName val="TruckingHourlyCost"/>
-      <sheetName val="TruckingTime"/>
-      <sheetName val="DisposalExpansionCost"/>
-      <sheetName val="DisposalCapacityIncrements"/>
-      <sheetName val="StorageExpansionCost"/>
-      <sheetName val="StorageCapacityIncrements"/>
-      <sheetName val="TreatmentExpansionCost"/>
-      <sheetName val="TreatmentCapacityIncrements"/>
-      <sheetName val="PipelineCapexDistanceBased"/>
-      <sheetName val="PipelineExpansionDistance"/>
-      <sheetName val="PipelineCapexCapacityBased"/>
-      <sheetName val="PipelineCapacityIncrements"/>
-      <sheetName val="PipelineDiameterValues"/>
-      <sheetName val="TreatmentEfficiency"/>
-      <sheetName val="RemovalEfficiency"/>
-      <sheetName val="DesalinationTechnologies"/>
-      <sheetName val="DesalinationSites"/>
-      <sheetName val="BeneficialReuseCost"/>
-      <sheetName val="BeneficialReuseCredit"/>
-      <sheetName val="CompletionsPadOutsideSystem"/>
-      <sheetName val="Hydraulics"/>
-      <sheetName val="Economics"/>
-      <sheetName val="ExternalWaterQuality"/>
-      <sheetName val="PadWaterQuality"/>
-      <sheetName val="StorageInitialWaterQuality"/>
-      <sheetName val="AirEmissionCoefficients"/>
-      <sheetName val="TreatmentEmissionCoefficients"/>
-      <sheetName val="PadStorageInitialWaterQuality"/>
-      <sheetName val="TreatmentExpansionLeadTime"/>
-      <sheetName val="DisposalExpansionLeadTime"/>
-      <sheetName val="StorageExpansionLeadTime"/>
-      <sheetName val="PipelineExpansionLeadTime_Dist"/>
-      <sheetName val="PipelineExpansionLeadTime_Capac"/>
-      <sheetName val="SWDDeep"/>
-      <sheetName val="SWDAveragePressure"/>
-      <sheetName val="SWDProxPAWell"/>
-      <sheetName val="SWDProxInactiveWell"/>
-      <sheetName val="SWDProxEQ"/>
-      <sheetName val="SWDProxFault"/>
-      <sheetName val="SWDProxHpOrLpWell"/>
-      <sheetName val="SWDRiskFactors"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2">
-        <row r="2">
-          <cell r="A2" t="str">
-            <v>INDEX</v>
-          </cell>
-          <cell r="B2" t="str">
-            <v>VALUE</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3" t="str">
-            <v>volume</v>
-          </cell>
-          <cell r="B3" t="str">
-            <v>bbl</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4" t="str">
-            <v>distance</v>
-          </cell>
-          <cell r="B4" t="str">
-            <v>mile</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5" t="str">
-            <v>diameter</v>
-          </cell>
-          <cell r="B5" t="str">
-            <v>inch</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6" t="str">
-            <v>concentration</v>
-          </cell>
-          <cell r="B6" t="str">
-            <v>mg/liter</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7" t="str">
-            <v>currency</v>
-          </cell>
-          <cell r="B7" t="str">
-            <v>USD</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8" t="str">
-            <v>time</v>
-          </cell>
-          <cell r="B8" t="str">
-            <v>day</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9" t="str">
-            <v>pressure</v>
-          </cell>
-          <cell r="B9" t="str">
-            <v>psi</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10" t="str">
-            <v>elevation</v>
-          </cell>
-          <cell r="B10" t="str">
-            <v>foot</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11" t="str">
-            <v>decision period</v>
-          </cell>
-          <cell r="B11" t="str">
-            <v>week</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12" t="str">
-            <v>mass</v>
-          </cell>
-          <cell r="B12" t="str">
-            <v>g</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
-      <sheetData sheetId="27"/>
-      <sheetData sheetId="28"/>
-      <sheetData sheetId="29"/>
-      <sheetData sheetId="30"/>
-      <sheetData sheetId="31"/>
-      <sheetData sheetId="32"/>
-      <sheetData sheetId="33"/>
-      <sheetData sheetId="34"/>
-      <sheetData sheetId="35"/>
-      <sheetData sheetId="36"/>
-      <sheetData sheetId="37"/>
-      <sheetData sheetId="38"/>
-      <sheetData sheetId="39"/>
-      <sheetData sheetId="40"/>
-      <sheetData sheetId="41"/>
-      <sheetData sheetId="42"/>
-      <sheetData sheetId="43"/>
-      <sheetData sheetId="44"/>
-      <sheetData sheetId="45"/>
-      <sheetData sheetId="46"/>
-      <sheetData sheetId="47"/>
-      <sheetData sheetId="48"/>
-      <sheetData sheetId="49"/>
-      <sheetData sheetId="50"/>
-      <sheetData sheetId="51"/>
-      <sheetData sheetId="52"/>
-      <sheetData sheetId="53"/>
-      <sheetData sheetId="54"/>
-      <sheetData sheetId="55"/>
-      <sheetData sheetId="56"/>
-      <sheetData sheetId="57"/>
-      <sheetData sheetId="58"/>
-      <sheetData sheetId="59"/>
-      <sheetData sheetId="60"/>
-      <sheetData sheetId="61"/>
-      <sheetData sheetId="62"/>
-      <sheetData sheetId="63"/>
-      <sheetData sheetId="64"/>
-      <sheetData sheetId="65"/>
-      <sheetData sheetId="66"/>
-      <sheetData sheetId="67"/>
-      <sheetData sheetId="68"/>
-      <sheetData sheetId="69"/>
-      <sheetData sheetId="70"/>
-      <sheetData sheetId="71"/>
-      <sheetData sheetId="72"/>
-      <sheetData sheetId="73"/>
-      <sheetData sheetId="74"/>
-      <sheetData sheetId="75"/>
-      <sheetData sheetId="76"/>
-      <sheetData sheetId="77"/>
-      <sheetData sheetId="78"/>
-      <sheetData sheetId="79"/>
-      <sheetData sheetId="80"/>
-      <sheetData sheetId="81"/>
-      <sheetData sheetId="82"/>
-      <sheetData sheetId="83"/>
-      <sheetData sheetId="84"/>
-      <sheetData sheetId="85"/>
-      <sheetData sheetId="86"/>
-      <sheetData sheetId="87"/>
-      <sheetData sheetId="88"/>
-      <sheetData sheetId="89"/>
-      <sheetData sheetId="90"/>
-      <sheetData sheetId="91"/>
-      <sheetData sheetId="92"/>
-      <sheetData sheetId="93"/>
-      <sheetData sheetId="94"/>
-      <sheetData sheetId="95"/>
-      <sheetData sheetId="96"/>
-      <sheetData sheetId="97"/>
-      <sheetData sheetId="98"/>
-      <sheetData sheetId="99"/>
-      <sheetData sheetId="100"/>
-      <sheetData sheetId="101"/>
-      <sheetData sheetId="102"/>
-      <sheetData sheetId="103"/>
-      <sheetData sheetId="104"/>
-      <sheetData sheetId="105"/>
-      <sheetData sheetId="106"/>
-      <sheetData sheetId="107"/>
-      <sheetData sheetId="108"/>
-      <sheetData sheetId="109"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
@@ -2338,7 +2030,7 @@
   </sheetPr>
   <dimension ref="B1:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -16889,7 +16581,7 @@
   <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A2:A4"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17086,7 +16778,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17127,9 +16819,8 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="21" t="str">
-        <f>_xlfn.CONCAT("Trucking [", VLOOKUP("mass", [1]Units!A2:B12, 2, FALSE), "/hour]")</f>
-        <v>Trucking [g/hour]</v>
+      <c r="A3" s="21" t="s">
+        <v>293</v>
       </c>
       <c r="B3" s="67">
         <v>2035000</v>
@@ -17148,9 +16839,8 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="21" t="str">
-        <f>_xlfn.CONCAT("Pipeline Operations [", VLOOKUP("mass", [1]Units!A2:B12, 2, FALSE), "/(", VLOOKUP("volume", [1]Units!A2:B12, 2, FALSE), "*", VLOOKUP("distance", [1]Units!A2:B12, 2, FALSE), ")]")</f>
-        <v>Pipeline Operations [g/(bbl*mile)]</v>
+      <c r="A4" s="21" t="s">
+        <v>294</v>
       </c>
       <c r="B4" s="67">
         <v>22</v>
@@ -17169,9 +16859,8 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="21" t="str">
-        <f>_xlfn.CONCAT("Pipeline Installation [", VLOOKUP("mass", [1]Units!A2:B12, 2, FALSE), "/", VLOOKUP("distance", [1]Units!A2:B12, 2, FALSE), "]")</f>
-        <v>Pipeline Installation [g/mile]</v>
+      <c r="A5" s="21" t="s">
+        <v>295</v>
       </c>
       <c r="B5" s="67">
         <v>310000000</v>
@@ -17190,9 +16879,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="21" t="str">
-        <f>_xlfn.CONCAT("Disposal [", VLOOKUP("mass", [1]Units!A2:B12, 2, FALSE), "/", VLOOKUP("volume", [1]Units!A2:B12, 2, FALSE), "]")</f>
-        <v>Disposal [g/bbl]</v>
+      <c r="A6" s="21" t="s">
+        <v>296</v>
       </c>
       <c r="B6" s="67">
         <v>970</v>
@@ -17211,9 +16899,8 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="str">
-        <f>_xlfn.CONCAT("Storage [", VLOOKUP("mass", [1]Units!A2:B12, 2, FALSE), "/(", VLOOKUP("volume", [1]Units!A2:B12, 2, FALSE), "*", VLOOKUP("decision period", [1]Units!A2:B12, 2, FALSE), ")]")</f>
-        <v>Storage [g/(bbl*week)]</v>
+      <c r="A7" s="22" t="s">
+        <v>297</v>
       </c>
       <c r="B7" s="70">
         <v>1000</v>
@@ -17244,8 +16931,8 @@
   </sheetPr>
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17254,9 +16941,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT("Table of Air Emissions Coefficients for Treatment Technologies [", VLOOKUP("mass", [1]Units!A2:B12, 2, FALSE), "/", VLOOKUP("volume", [1]Units!A2:B12, 2, FALSE), "]")</f>
-        <v>Table of Air Emissions Coefficients for Treatment Technologies [g/bbl]</v>
+      <c r="A1" s="1" t="s">
+        <v>298</v>
       </c>
       <c r="B1" s="1"/>
     </row>

</xml_diff>

<commit_message>
update units in template
</commit_message>
<xml_diff>
--- a/backend/app/internal/assets/pareto_input_template.xlsx
+++ b/backend/app/internal/assets/pareto_input_template.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelpesce/Desktop/pareto-ui/backend/app/internal/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD92D4FB-1F95-F14E-9425-0AFBC6AD6077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF01FE4-DBFA-B94C-B276-A208E601EED8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="21560" windowHeight="18900" tabRatio="953" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="12340" yWindow="760" windowWidth="21560" windowHeight="18900" tabRatio="953" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
     <sheet name="Schematic" sheetId="82" r:id="rId2"/>
-    <sheet name="Units" sheetId="103" r:id="rId3"/>
+    <sheet name="Units" sheetId="150" r:id="rId3"/>
     <sheet name="ProductionPads" sheetId="1" r:id="rId4"/>
     <sheet name="ProductionTanks" sheetId="34" state="hidden" r:id="rId5"/>
     <sheet name="CompletionsPads" sheetId="3" r:id="rId6"/>
@@ -124,9 +124,6 @@
     <sheet name="SWDProxHpOrLpWell" sheetId="143" r:id="rId109"/>
     <sheet name="SWDRiskFactors" sheetId="146" r:id="rId110"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId111"/>
-  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="78" hidden="1">#REF!</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">TreatmentTechnologies!$A$1:$A$5</definedName>
@@ -153,7 +150,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="845" uniqueCount="306">
   <si>
     <t>Data Input Spreadsheet Overview</t>
   </si>
@@ -1056,6 +1053,21 @@
   </si>
   <si>
     <t>List of all Air Emissions Components [-]</t>
+  </si>
+  <si>
+    <t>1000g</t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>Mass units is used for measuring emissions coefficients (e.g. 10g per treated produced water bbl).</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>mass</t>
   </si>
 </sst>
 </file>
@@ -1528,7 +1540,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1714,9 +1726,6 @@
     <xf numFmtId="2" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1744,321 +1753,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Overview"/>
-      <sheetName val="Schematic"/>
-      <sheetName val="Units"/>
-      <sheetName val="ProductionPads"/>
-      <sheetName val="ProductionTanks"/>
-      <sheetName val="CompletionsPads"/>
-      <sheetName val="SWDSites"/>
-      <sheetName val="ExternalWaterSources"/>
-      <sheetName val="WaterQualityComponents"/>
-      <sheetName val="AirEmissionsComponents"/>
-      <sheetName val="StorageSites"/>
-      <sheetName val="TreatmentSites"/>
-      <sheetName val="TreatmentTechnologies"/>
-      <sheetName val="ReuseOptions"/>
-      <sheetName val="NetworkNodes"/>
-      <sheetName val="PipelineDiameters"/>
-      <sheetName val="StorageCapacities"/>
-      <sheetName val="TreatmentCapacities"/>
-      <sheetName val="InjectionCapacities"/>
-      <sheetName val="PNA"/>
-      <sheetName val="CNA"/>
-      <sheetName val="CCA"/>
-      <sheetName val="NNA"/>
-      <sheetName val="NCA"/>
-      <sheetName val="NKA"/>
-      <sheetName val="NRA"/>
-      <sheetName val="NSA"/>
-      <sheetName val="NOA"/>
-      <sheetName val="SNA"/>
-      <sheetName val="SOA"/>
-      <sheetName val="FCA"/>
-      <sheetName val="RCA"/>
-      <sheetName val="RSA"/>
-      <sheetName val="SCA"/>
-      <sheetName val="RNA"/>
-      <sheetName val="ROA"/>
-      <sheetName val="RKA"/>
-      <sheetName val="PCT"/>
-      <sheetName val="FCT"/>
-      <sheetName val="PKT"/>
-      <sheetName val="CKT"/>
-      <sheetName val="CCT"/>
-      <sheetName val="CST"/>
-      <sheetName val="RST"/>
-      <sheetName val="ROT"/>
-      <sheetName val="SOT"/>
-      <sheetName val="RKT"/>
-      <sheetName val="Elevation"/>
-      <sheetName val="CompletionsDemand"/>
-      <sheetName val="PadRates"/>
-      <sheetName val="FlowbackRates"/>
-      <sheetName val="WellPressure"/>
-      <sheetName val="InitialPipelineCapacity"/>
-      <sheetName val="InitialPipelineDiameters"/>
-      <sheetName val="InitialDisposalCapacity"/>
-      <sheetName val="InitialStorageCapacity"/>
-      <sheetName val="InitialTreatmentCapacity"/>
-      <sheetName val="ReuseMinimum"/>
-      <sheetName val="ReuseCapacity"/>
-      <sheetName val="ExtWaterSourcingAvailability"/>
-      <sheetName val="CompletionsPadStorage"/>
-      <sheetName val="PadOffloadingCapacity"/>
-      <sheetName val="NodeCapacities"/>
-      <sheetName val="DisposalOperatingCapacity"/>
-      <sheetName val="DisposalOperationalCost"/>
-      <sheetName val="TreatmentOperationalCost"/>
-      <sheetName val="ReuseOperationalCost"/>
-      <sheetName val="PipelineOperationalCost"/>
-      <sheetName val="ExternalSourcingCost"/>
-      <sheetName val="TruckingHourlyCost"/>
-      <sheetName val="TruckingTime"/>
-      <sheetName val="DisposalExpansionCost"/>
-      <sheetName val="DisposalCapacityIncrements"/>
-      <sheetName val="StorageExpansionCost"/>
-      <sheetName val="StorageCapacityIncrements"/>
-      <sheetName val="TreatmentExpansionCost"/>
-      <sheetName val="TreatmentCapacityIncrements"/>
-      <sheetName val="PipelineCapexDistanceBased"/>
-      <sheetName val="PipelineExpansionDistance"/>
-      <sheetName val="PipelineCapexCapacityBased"/>
-      <sheetName val="PipelineCapacityIncrements"/>
-      <sheetName val="PipelineDiameterValues"/>
-      <sheetName val="TreatmentEfficiency"/>
-      <sheetName val="RemovalEfficiency"/>
-      <sheetName val="DesalinationTechnologies"/>
-      <sheetName val="DesalinationSites"/>
-      <sheetName val="BeneficialReuseCost"/>
-      <sheetName val="BeneficialReuseCredit"/>
-      <sheetName val="CompletionsPadOutsideSystem"/>
-      <sheetName val="Hydraulics"/>
-      <sheetName val="Economics"/>
-      <sheetName val="ExternalWaterQuality"/>
-      <sheetName val="PadWaterQuality"/>
-      <sheetName val="StorageInitialWaterQuality"/>
-      <sheetName val="AirEmissionCoefficients"/>
-      <sheetName val="TreatmentEmissionCoefficients"/>
-      <sheetName val="PadStorageInitialWaterQuality"/>
-      <sheetName val="TreatmentExpansionLeadTime"/>
-      <sheetName val="DisposalExpansionLeadTime"/>
-      <sheetName val="StorageExpansionLeadTime"/>
-      <sheetName val="PipelineExpansionLeadTime_Dist"/>
-      <sheetName val="PipelineExpansionLeadTime_Capac"/>
-      <sheetName val="SWDDeep"/>
-      <sheetName val="SWDAveragePressure"/>
-      <sheetName val="SWDProxPAWell"/>
-      <sheetName val="SWDProxInactiveWell"/>
-      <sheetName val="SWDProxEQ"/>
-      <sheetName val="SWDProxFault"/>
-      <sheetName val="SWDProxHpOrLpWell"/>
-      <sheetName val="SWDRiskFactors"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2">
-        <row r="2">
-          <cell r="A2" t="str">
-            <v>INDEX</v>
-          </cell>
-          <cell r="B2" t="str">
-            <v>VALUE</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3" t="str">
-            <v>volume</v>
-          </cell>
-          <cell r="B3" t="str">
-            <v>bbl</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4" t="str">
-            <v>distance</v>
-          </cell>
-          <cell r="B4" t="str">
-            <v>mile</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5" t="str">
-            <v>diameter</v>
-          </cell>
-          <cell r="B5" t="str">
-            <v>inch</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6" t="str">
-            <v>concentration</v>
-          </cell>
-          <cell r="B6" t="str">
-            <v>mg/liter</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7" t="str">
-            <v>currency</v>
-          </cell>
-          <cell r="B7" t="str">
-            <v>USD</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8" t="str">
-            <v>time</v>
-          </cell>
-          <cell r="B8" t="str">
-            <v>day</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9" t="str">
-            <v>pressure</v>
-          </cell>
-          <cell r="B9" t="str">
-            <v>psi</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10" t="str">
-            <v>elevation</v>
-          </cell>
-          <cell r="B10" t="str">
-            <v>foot</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11" t="str">
-            <v>decision period</v>
-          </cell>
-          <cell r="B11" t="str">
-            <v>week</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
-      <sheetData sheetId="27"/>
-      <sheetData sheetId="28"/>
-      <sheetData sheetId="29"/>
-      <sheetData sheetId="30"/>
-      <sheetData sheetId="31"/>
-      <sheetData sheetId="32"/>
-      <sheetData sheetId="33"/>
-      <sheetData sheetId="34"/>
-      <sheetData sheetId="35"/>
-      <sheetData sheetId="36"/>
-      <sheetData sheetId="37"/>
-      <sheetData sheetId="38"/>
-      <sheetData sheetId="39"/>
-      <sheetData sheetId="40"/>
-      <sheetData sheetId="41"/>
-      <sheetData sheetId="42"/>
-      <sheetData sheetId="43"/>
-      <sheetData sheetId="44"/>
-      <sheetData sheetId="45"/>
-      <sheetData sheetId="46"/>
-      <sheetData sheetId="47"/>
-      <sheetData sheetId="48"/>
-      <sheetData sheetId="49"/>
-      <sheetData sheetId="50"/>
-      <sheetData sheetId="51"/>
-      <sheetData sheetId="52"/>
-      <sheetData sheetId="53"/>
-      <sheetData sheetId="54"/>
-      <sheetData sheetId="55"/>
-      <sheetData sheetId="56"/>
-      <sheetData sheetId="57"/>
-      <sheetData sheetId="58"/>
-      <sheetData sheetId="59"/>
-      <sheetData sheetId="60"/>
-      <sheetData sheetId="61"/>
-      <sheetData sheetId="62"/>
-      <sheetData sheetId="63"/>
-      <sheetData sheetId="64"/>
-      <sheetData sheetId="65"/>
-      <sheetData sheetId="66"/>
-      <sheetData sheetId="67"/>
-      <sheetData sheetId="68"/>
-      <sheetData sheetId="69"/>
-      <sheetData sheetId="70"/>
-      <sheetData sheetId="71"/>
-      <sheetData sheetId="72"/>
-      <sheetData sheetId="73"/>
-      <sheetData sheetId="74"/>
-      <sheetData sheetId="75"/>
-      <sheetData sheetId="76"/>
-      <sheetData sheetId="77"/>
-      <sheetData sheetId="78"/>
-      <sheetData sheetId="79"/>
-      <sheetData sheetId="80"/>
-      <sheetData sheetId="81"/>
-      <sheetData sheetId="82"/>
-      <sheetData sheetId="83"/>
-      <sheetData sheetId="84"/>
-      <sheetData sheetId="85"/>
-      <sheetData sheetId="86"/>
-      <sheetData sheetId="87"/>
-      <sheetData sheetId="88"/>
-      <sheetData sheetId="89"/>
-      <sheetData sheetId="90"/>
-      <sheetData sheetId="91"/>
-      <sheetData sheetId="92"/>
-      <sheetData sheetId="93"/>
-      <sheetData sheetId="94"/>
-      <sheetData sheetId="95"/>
-      <sheetData sheetId="96"/>
-      <sheetData sheetId="97"/>
-      <sheetData sheetId="98"/>
-      <sheetData sheetId="99"/>
-      <sheetData sheetId="100"/>
-      <sheetData sheetId="101"/>
-      <sheetData sheetId="102"/>
-      <sheetData sheetId="103"/>
-      <sheetData sheetId="104"/>
-      <sheetData sheetId="105"/>
-      <sheetData sheetId="106"/>
-      <sheetData sheetId="107"/>
-      <sheetData sheetId="108"/>
-      <sheetData sheetId="109"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2976,9 +2670,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Storage Expansion Lead Time [",VLOOKUP("decision period", Units!$A$2:$B$11, 2, FALSE),"s]")</f>
-        <v>Table of Storage Expansion Lead Time [weeks]</v>
+      <c r="A1" s="1" t="e">
+        <f>_xlfn.CONCAT( "Table of Storage Expansion Lead Time [",VLOOKUP("decision period",#REF!, 2, FALSE),"s]")</f>
+        <v>#REF!</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -3033,9 +2727,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Pipeline Expansion Lead Time - Distance Based [",VLOOKUP("decision period", Units!$A$2:$B$11, 2, FALSE),"s/",VLOOKUP("distance", Units!$A$2:$B$11, 2, FALSE),"]")</f>
-        <v>Table of Pipeline Expansion Lead Time - Distance Based [weeks/mile]</v>
+      <c r="A1" s="1" t="e">
+        <f>_xlfn.CONCAT( "Table of Pipeline Expansion Lead Time - Distance Based [",VLOOKUP("decision period",#REF!, 2, FALSE),"s/",VLOOKUP("distance",#REF!, 2, FALSE),"]")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -3071,9 +2765,9 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Pipeline Expansion Lead Time - Capacity Based [",VLOOKUP("decision period", Units!$A$2:$B$11, 2, FALSE),"s]")</f>
-        <v>Table of Pipeline Expansion Lead Time - Capacity Based [weeks]</v>
+      <c r="A1" s="1" t="e">
+        <f>_xlfn.CONCAT( "Table of Pipeline Expansion Lead Time - Capacity Based [",VLOOKUP("decision period",#REF!, 2, FALSE),"s]")</f>
+        <v>#REF!</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -4890,15 +4584,13 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FEB10CD-C2F5-4A5B-9D35-9BA20FBC12B6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6F19DE1-7232-9D4E-A12D-8B7450D54C2A}">
   <sheetPr>
     <tabColor theme="2" tint="-9.9978637043366805E-2"/>
   </sheetPr>
-  <dimension ref="A1:BA12"/>
+  <dimension ref="A1:BB12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4922,12 +4614,12 @@
     <col min="54" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:54" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:53" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:54" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>44</v>
       </c>
@@ -4947,7 +4639,7 @@
       <c r="J2" s="43"/>
       <c r="K2" s="45"/>
     </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
         <v>48</v>
       </c>
@@ -4977,7 +4669,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A4" s="21" t="s">
         <v>55</v>
       </c>
@@ -5001,7 +4693,7 @@
       <c r="J4" s="33"/>
       <c r="K4" s="35"/>
     </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A5" s="21" t="s">
         <v>60</v>
       </c>
@@ -5019,7 +4711,7 @@
       <c r="J5" s="34"/>
       <c r="K5" s="36"/>
     </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A6" s="21" t="s">
         <v>63</v>
       </c>
@@ -5043,7 +4735,7 @@
       <c r="J6" s="34"/>
       <c r="K6" s="36"/>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A7" s="21" t="s">
         <v>67</v>
       </c>
@@ -5067,7 +4759,7 @@
       <c r="J7" s="34"/>
       <c r="K7" s="36"/>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A8" s="21" t="s">
         <v>72</v>
       </c>
@@ -5109,7 +4801,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A9" s="21" t="s">
         <v>233</v>
       </c>
@@ -5157,7 +4849,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" x14ac:dyDescent="0.2">
       <c r="A10" s="21" t="s">
         <v>238</v>
       </c>
@@ -5199,33 +4891,33 @@
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="1:53" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
+    <row r="11" spans="1:54" x14ac:dyDescent="0.2">
+      <c r="A11" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="D11" s="42" t="s">
+      <c r="D11" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="E11" s="46" t="s">
+      <c r="E11" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="F11" s="47" t="s">
+      <c r="F11" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="G11" s="48" t="s">
+      <c r="G11" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="H11" s="42"/>
-      <c r="I11" s="49" t="s">
+      <c r="H11" s="38"/>
+      <c r="I11" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="J11" s="47" t="s">
+      <c r="J11" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="K11" s="48" t="s">
+      <c r="K11" s="36" t="s">
         <v>82</v>
       </c>
       <c r="AU11" s="1" t="s">
@@ -5235,39 +4927,61 @@
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:54" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="22" t="s">
+        <v>305</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>304</v>
+      </c>
+      <c r="D12" s="42" t="s">
+        <v>303</v>
+      </c>
+      <c r="E12" s="46" t="s">
+        <v>302</v>
+      </c>
+      <c r="F12" s="47" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" s="48" t="s">
+        <v>301</v>
+      </c>
+      <c r="H12" s="42"/>
+      <c r="I12" s="49"/>
+      <c r="J12" s="47"/>
+      <c r="K12" s="48"/>
       <c r="AU12" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="BA12" s="1" t="s">
+      <c r="BB12" s="1" t="s">
         <v>81</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="8">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{0221D16C-ACF3-42AE-9C26-25DCEE5A4935}">
-      <formula1>$AT$9:$AT$10</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11" xr:uid="{F2F718D3-1F2B-4B75-B6F1-E58F1982C8E5}">
+      <formula1>$BA$9:$BA$12</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9" xr:uid="{A9C3EE24-05FB-48EE-9886-7F2676DC7EE9}">
+      <formula1>$AZ$9:$AZ$10</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{C77CFCD0-E9B6-4035-9AEC-88575ADC24B9}">
+      <formula1>$AV$9:$AV$10</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8" xr:uid="{C12D334A-9947-4F69-ADBA-610C067372DB}">
+      <formula1>$AY$9:$AY$10</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7" xr:uid="{786B06B2-2E18-4E07-817C-AFF8EF08A5C5}">
+      <formula1>$AX$9:$AX$10</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{9028AD91-E96A-4D2A-B2A3-6F94739A937D}">
+      <formula1>$AW$9:$AW$10</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 B10" xr:uid="{48F5BE7D-5F59-4B5D-A488-104864EC18E3}">
       <formula1>$AU$9:$AU$12</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{9028AD91-E96A-4D2A-B2A3-6F94739A937D}">
-      <formula1>$AW$9:$AW$10</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7" xr:uid="{786B06B2-2E18-4E07-817C-AFF8EF08A5C5}">
-      <formula1>$AX$9:$AX$10</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8" xr:uid="{C12D334A-9947-4F69-ADBA-610C067372DB}">
-      <formula1>$AY$9:$AY$10</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5" xr:uid="{C77CFCD0-E9B6-4035-9AEC-88575ADC24B9}">
-      <formula1>$AV$9:$AV$10</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9" xr:uid="{A9C3EE24-05FB-48EE-9886-7F2676DC7EE9}">
-      <formula1>$AZ$9:$AZ$10</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11" xr:uid="{F2F718D3-1F2B-4B75-B6F1-E58F1982C8E5}">
-      <formula1>$BA$9:$BA$12</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{0221D16C-ACF3-42AE-9C26-25DCEE5A4935}">
+      <formula1>$AT$9:$AT$10</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6260,9 +5974,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:55" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Completions Water Demand for Completions Sites over ",VLOOKUP("decision period", Units!$A$2:$B$11, 2, FALSE),"s [",VLOOKUP("volume", Units!$A$2:$B$11, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$11, 2, FALSE),"]")</f>
-        <v>Table of Completions Water Demand for Completions Sites over weeks [bbl/day]</v>
+      <c r="A1" s="1" t="e">
+        <f>_xlfn.CONCAT( "Table of Completions Water Demand for Completions Sites over ",VLOOKUP("decision period",#REF!, 2, FALSE),"s [",VLOOKUP("volume",#REF!, 2, FALSE),"/", VLOOKUP("time",#REF!, 2, FALSE),"]")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="2" spans="1:55" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -6569,9 +6283,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Production Rate Forecasts by Pads [",VLOOKUP("volume", Units!$A$2:$B$11, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$11, 2, FALSE),"]")</f>
-        <v>Table of Production Rate Forecasts by Pads [bbl/day]</v>
+      <c r="A1" s="1" t="e">
+        <f>_xlfn.CONCAT( "Table of Production Rate Forecasts by Pads [",VLOOKUP("volume",#REF!, 2, FALSE),"/", VLOOKUP("time",#REF!, 2, FALSE),"]")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="2" spans="1:53" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -6992,9 +6706,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Flowback Rate Forecasts by Pads [",VLOOKUP("volume", Units!$A$2:$B$11, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$11, 2, FALSE),"]")</f>
-        <v>Table of Flowback Rate Forecasts by Pads [bbl/day]</v>
+      <c r="A1" s="1" t="e">
+        <f>_xlfn.CONCAT( "Table of Flowback Rate Forecasts by Pads [",VLOOKUP("volume",#REF!, 2, FALSE),"/", VLOOKUP("time",#REF!, 2, FALSE),"]")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="2" spans="1:53" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -8409,9 +8123,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Initial Pipeline Capacity between Sites [",VLOOKUP("volume", Units!$A$2:$B$11, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$11, 2, FALSE),"]")</f>
-        <v>Table of Initial Pipeline Capacity between Sites [bbl/day]</v>
+      <c r="A1" s="1" t="e">
+        <f>_xlfn.CONCAT( "Table of Initial Pipeline Capacity between Sites [",VLOOKUP("volume",#REF!, 2, FALSE),"/", VLOOKUP("time",#REF!, 2, FALSE),"]")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
@@ -12949,9 +12663,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Initial Disposal Capacity [",VLOOKUP("volume", Units!$A$2:$B$11, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$11, 2, FALSE),"]")</f>
-        <v>Table of Initial Disposal Capacity [bbl/day]</v>
+      <c r="A1" s="1" t="e">
+        <f>_xlfn.CONCAT( "Table of Initial Disposal Capacity [",VLOOKUP("volume",#REF!, 2, FALSE),"/", VLOOKUP("time",#REF!, 2, FALSE),"]")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -12992,9 +12706,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Initial Storage Capacity [",VLOOKUP("volume", Units!$A$2:$B$11, 2, FALSE),"]")</f>
-        <v>Table of Initial Storage Capacity [bbl]</v>
+      <c r="A1" s="1" t="e">
+        <f>_xlfn.CONCAT( "Table of Initial Storage Capacity [",VLOOKUP("volume",#REF!, 2, FALSE),"]")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -13039,9 +12753,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Initial Treatment Capacity [",VLOOKUP("volume", Units!$A$2:$B$11, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$11, 2, FALSE),"]")</f>
-        <v>Table of Initial Treatment Capacity [bbl/day]</v>
+      <c r="A1" s="1" t="e">
+        <f>_xlfn.CONCAT( "Table of Initial Treatment Capacity [",VLOOKUP("volume",#REF!, 2, FALSE),"/", VLOOKUP("time",#REF!, 2, FALSE),"]")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -13092,9 +12806,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Beneficial Reuse minimum required flow [",VLOOKUP("volume", Units!$A$2:$B$11, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$11, 2, FALSE),"]")</f>
-        <v>Table of Beneficial Reuse minimum required flow [bbl/day]</v>
+      <c r="A1" s="1" t="e">
+        <f>_xlfn.CONCAT( "Table of Beneficial Reuse minimum required flow [",VLOOKUP("volume",#REF!, 2, FALSE),"/", VLOOKUP("time",#REF!, 2, FALSE),"]")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="2" spans="1:53" x14ac:dyDescent="0.2">
@@ -13444,9 +13158,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Beneficial Reuse Capacity [",VLOOKUP("volume", Units!$A$2:$B$11, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$11, 2, FALSE),"] (leave cells blank to indicate infinite capacity)")</f>
-        <v>Table of Beneficial Reuse Capacity [bbl/day] (leave cells blank to indicate infinite capacity)</v>
+      <c r="A1" s="1" t="e">
+        <f>_xlfn.CONCAT( "Table of Beneficial Reuse Capacity [",VLOOKUP("volume",#REF!, 2, FALSE),"/", VLOOKUP("time",#REF!, 2, FALSE),"] (leave cells blank to indicate infinite capacity)")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="2" spans="1:53" x14ac:dyDescent="0.2">
@@ -13846,9 +13560,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of External Water Sourcing Availability [",VLOOKUP("volume", Units!$A$2:$B$11, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$11, 2, FALSE),"]")</f>
-        <v>Table of External Water Sourcing Availability [bbl/day]</v>
+      <c r="A1" s="1" t="e">
+        <f>_xlfn.CONCAT( "Table of External Water Sourcing Availability [",VLOOKUP("volume",#REF!, 2, FALSE),"/", VLOOKUP("time",#REF!, 2, FALSE),"]")</f>
+        <v>#REF!</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>105</v>
@@ -14167,9 +13881,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Completions Pad Storage Capacity [",VLOOKUP("volume", Units!$A$2:$B$11, 2, FALSE),"]")</f>
-        <v>Table of Completions Pad Storage Capacity [bbl]</v>
+      <c r="A1" s="1" t="e">
+        <f>_xlfn.CONCAT( "Table of Completions Pad Storage Capacity [",VLOOKUP("volume",#REF!, 2, FALSE),"]")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -14206,9 +13920,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Pad Offloading Capacity [",VLOOKUP("volume", Units!$A$2:$B$11, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$11, 2, FALSE),"]")</f>
-        <v>Table of Pad Offloading Capacity [bbl/day]</v>
+      <c r="A1" s="1" t="e">
+        <f>_xlfn.CONCAT( "Table of Pad Offloading Capacity [",VLOOKUP("volume",#REF!, 2, FALSE),"/", VLOOKUP("time",#REF!, 2, FALSE),"]")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -14246,9 +13960,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Node Capacity Capacity [",VLOOKUP("volume", Units!$A$2:$B$11, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$11, 2, FALSE),"]", " *absence of node or empty cell signifies no max capacity")</f>
-        <v>Table of Node Capacity Capacity [bbl/day] *absence of node or empty cell signifies no max capacity</v>
+      <c r="A1" s="1" t="e">
+        <f>_xlfn.CONCAT( "Table of Node Capacity Capacity [",VLOOKUP("volume",#REF!, 2, FALSE),"/", VLOOKUP("time",#REF!, 2, FALSE),"]", " *absence of node or empty cell signifies no max capacity")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -14526,9 +14240,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Disposal Operational Cost [",VLOOKUP("currency", Units!$A$2:$B$11, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$11, 2, FALSE),"]")</f>
-        <v>Table of Disposal Operational Cost [USD/bbl]</v>
+      <c r="A1" s="1" t="e">
+        <f>_xlfn.CONCAT( "Table of Disposal Operational Cost [",VLOOKUP("currency",#REF!, 2, FALSE),"/", VLOOKUP("volume",#REF!, 2, FALSE),"]")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -14569,9 +14283,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Treatment Operational Cost [",VLOOKUP("currency", Units!$A$2:$B$11, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$11, 2, FALSE),"]")</f>
-        <v>Table of Treatment Operational Cost [USD/bbl]</v>
+      <c r="A1" s="1" t="e">
+        <f>_xlfn.CONCAT( "Table of Treatment Operational Cost [",VLOOKUP("currency",#REF!, 2, FALSE),"/", VLOOKUP("volume",#REF!, 2, FALSE),"]")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -14657,9 +14371,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Reuse Operational Cost [",VLOOKUP("currency", Units!$A$2:$B$11, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$11, 2, FALSE),"]")</f>
-        <v>Table of Reuse Operational Cost [USD/bbl]</v>
+      <c r="A1" s="1" t="e">
+        <f>_xlfn.CONCAT( "Table of Reuse Operational Cost [",VLOOKUP("currency",#REF!, 2, FALSE),"/", VLOOKUP("volume",#REF!, 2, FALSE),"]")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -14696,9 +14410,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Pipeline Operational Cost between Sites [",VLOOKUP("currency", Units!$A$2:$B$11, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$11, 2, FALSE),"]")</f>
-        <v>Table of Pipeline Operational Cost between Sites [USD/bbl]</v>
+      <c r="A1" s="1" t="e">
+        <f>_xlfn.CONCAT( "Table of Pipeline Operational Cost between Sites [",VLOOKUP("currency",#REF!, 2, FALSE),"/", VLOOKUP("volume",#REF!, 2, FALSE),"]")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
@@ -15234,9 +14948,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of External Water Souring Cost [",VLOOKUP("currency", Units!$A$2:$B$11, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$11, 2, FALSE),"]")</f>
-        <v>Table of External Water Souring Cost [USD/bbl]</v>
+      <c r="A1" s="1" t="e">
+        <f>_xlfn.CONCAT( "Table of External Water Souring Cost [",VLOOKUP("currency",#REF!, 2, FALSE),"/", VLOOKUP("volume",#REF!, 2, FALSE),"]")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -15323,9 +15037,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Trucking Hourly Cost [",VLOOKUP("currency", Units!$A$2:$B$11, 2, FALSE),"/", "hour","]")</f>
-        <v>Table of Trucking Hourly Cost [USD/hour]</v>
+      <c r="A1" s="1" t="e">
+        <f>_xlfn.CONCAT( "Table of Trucking Hourly Cost [",VLOOKUP("currency",#REF!, 2, FALSE),"/", "hour","]")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -15446,9 +15160,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Disposal Capacity Expansion Cost [",VLOOKUP("currency", Units!$A$2:$B$11, 2, FALSE),"/(", VLOOKUP("volume", Units!$A$2:$B$11, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$11, 2, FALSE),")]")</f>
-        <v>Table of Disposal Capacity Expansion Cost [USD/(bbl/day)]</v>
+      <c r="A1" s="1" t="e">
+        <f>_xlfn.CONCAT( "Table of Disposal Capacity Expansion Cost [",VLOOKUP("currency",#REF!, 2, FALSE),"/(", VLOOKUP("volume",#REF!, 2, FALSE),"/", VLOOKUP("time",#REF!, 2, FALSE),")]")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -15497,9 +15211,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Disposal Capacity Expansion Increments [",VLOOKUP("volume", Units!$A$2:$B$11, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$11, 2, FALSE),"]")</f>
-        <v>Table of Disposal Capacity Expansion Increments [bbl/day]</v>
+      <c r="A1" s="1" t="e">
+        <f>_xlfn.CONCAT( "Table of Disposal Capacity Expansion Increments [",VLOOKUP("volume",#REF!, 2, FALSE),"/", VLOOKUP("time",#REF!, 2, FALSE),"]")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -15548,9 +15262,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Storage Capacity Expansion Cost [",VLOOKUP("currency", Units!$A$2:$B$11, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$11, 2, FALSE),"]")</f>
-        <v>Table of Storage Capacity Expansion Cost [USD/bbl]</v>
+      <c r="A1" s="1" t="e">
+        <f>_xlfn.CONCAT( "Table of Storage Capacity Expansion Cost [",VLOOKUP("currency",#REF!, 2, FALSE),"/", VLOOKUP("volume",#REF!, 2, FALSE),"]")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -15605,9 +15319,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Storage Capacity Expansion Increments [",VLOOKUP("volume", Units!$A$2:$B$11, 2, FALSE),"]")</f>
-        <v>Table of Storage Capacity Expansion Increments [bbl]</v>
+      <c r="A1" s="1" t="e">
+        <f>_xlfn.CONCAT( "Table of Storage Capacity Expansion Increments [",VLOOKUP("volume",#REF!, 2, FALSE),"]")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -15657,9 +15371,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Treatment Capacity Expansion Cost [",VLOOKUP("currency", Units!$A$2:$B$11, 2, FALSE),"/(", VLOOKUP("volume", Units!$A$2:$B$11, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$11, 2, FALSE),")]")</f>
-        <v>Table of Treatment Capacity Expansion Cost [USD/(bbl/day)]</v>
+      <c r="A1" s="1" t="e">
+        <f>_xlfn.CONCAT( "Table of Treatment Capacity Expansion Cost [",VLOOKUP("currency",#REF!, 2, FALSE),"/(", VLOOKUP("volume",#REF!, 2, FALSE),"/", VLOOKUP("time",#REF!, 2, FALSE),")]")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -15778,9 +15492,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Treatment Capacity Expansion Increments [",VLOOKUP("volume", Units!$A$2:$B$11, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$11, 2, FALSE),"]")</f>
-        <v>Table of Treatment Capacity Expansion Increments [bbl/day]</v>
+      <c r="A1" s="1" t="e">
+        <f>_xlfn.CONCAT( "Table of Treatment Capacity Expansion Increments [",VLOOKUP("volume",#REF!, 2, FALSE),"/", VLOOKUP("time",#REF!, 2, FALSE),"]")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -15858,9 +15572,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Pipeline Expansion Cost [",VLOOKUP("currency", Units!$A$2:$B$11, 2, FALSE),"/(", VLOOKUP("diameter", Units!$A$2:$B$11, 2, FALSE),"-", VLOOKUP("distance", Units!$A$2:$B$11, 2, FALSE),")]")</f>
-        <v>Pipeline Expansion Cost [USD/(inch-mile)]</v>
+      <c r="A1" s="1" t="e">
+        <f>_xlfn.CONCAT( "Pipeline Expansion Cost [",VLOOKUP("currency",#REF!, 2, FALSE),"/(", VLOOKUP("diameter",#REF!, 2, FALSE),"-", VLOOKUP("distance",#REF!, 2, FALSE),")]")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -15903,9 +15617,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Pipeline Expansion Distances [",VLOOKUP("distance", Units!$A$2:$B$11, 2, FALSE),"]")</f>
-        <v>Table of Pipeline Expansion Distances [mile]</v>
+      <c r="A1" s="1" t="e">
+        <f>_xlfn.CONCAT( "Table of Pipeline Expansion Distances [",VLOOKUP("distance",#REF!, 2, FALSE),"]")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
@@ -16481,9 +16195,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Pipeline Capacity Expansion Costs [",VLOOKUP("currency", Units!$A$2:$B$11, 2, FALSE),"/(", VLOOKUP("volume", Units!$A$2:$B$11, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$11, 2, FALSE),")]")</f>
-        <v>Table of Pipeline Capacity Expansion Costs [USD/(bbl/day)]</v>
+      <c r="A1" s="1" t="e">
+        <f>_xlfn.CONCAT( "Table of Pipeline Capacity Expansion Costs [",VLOOKUP("currency",#REF!, 2, FALSE),"/(", VLOOKUP("volume",#REF!, 2, FALSE),"/", VLOOKUP("time",#REF!, 2, FALSE),")]")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -16541,9 +16255,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Pipeline Capacity Expansion Increments [",VLOOKUP("volume", Units!$A$2:$B$11, 2, FALSE),"/", VLOOKUP("time", Units!$A$2:$B$11, 2, FALSE),"]")</f>
-        <v>Table of Pipeline Capacity Expansion Increments [bbl/day]</v>
+      <c r="A1" s="1" t="e">
+        <f>_xlfn.CONCAT( "Table of Pipeline Capacity Expansion Increments [",VLOOKUP("volume",#REF!, 2, FALSE),"/", VLOOKUP("time",#REF!, 2, FALSE),"]")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -16616,9 +16330,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Pipeline Diameters [",VLOOKUP("diameter", Units!$A$2:$B$11, 2, FALSE),"]")</f>
-        <v>Table of Pipeline Diameters [inch]</v>
+      <c r="A1" s="1" t="e">
+        <f>_xlfn.CONCAT( "Table of Pipeline Diameters [",VLOOKUP("diameter",#REF!, 2, FALSE),"]")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -16977,9 +16691,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table with credit received for sending water to beneficial reuse [",VLOOKUP("currency", Units!$A$2:$B$11, 2, FALSE),"/", VLOOKUP("volume", Units!$A$2:$B$11, 2, FALSE),"]")</f>
-        <v>Table with credit received for sending water to beneficial reuse [USD/bbl]</v>
+      <c r="A1" s="1" t="e">
+        <f>_xlfn.CONCAT( "Table with credit received for sending water to beneficial reuse [",VLOOKUP("currency",#REF!, 2, FALSE),"/", VLOOKUP("volume",#REF!, 2, FALSE),"]")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -17219,25 +16933,25 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Water Quality of External Water Sources [",VLOOKUP("concentration", [1]Units!$A$2:$B$11, 2, FALSE),"]")</f>
+        <f>_xlfn.CONCAT( "Table of Water Quality of External Water Sources [",VLOOKUP("concentration", Units!$A$2:$B$11, 2, FALSE),"]")</f>
         <v>Table of Water Quality of External Water Sources [mg/liter]</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="6" t="s">
         <v>296</v>
       </c>
-      <c r="B2" s="81" t="s">
+      <c r="B2" s="6" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="81"/>
-      <c r="B3" s="82"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="81"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="81"/>
-      <c r="B4" s="82"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="81"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17268,9 +16982,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Water Quality of Produced Water and Flowback Water [",VLOOKUP("concentration", Units!$A$2:$B$11, 2, FALSE),"]")</f>
-        <v>Table of Water Quality of Produced Water and Flowback Water [mg/liter]</v>
+      <c r="A1" s="1" t="e">
+        <f>_xlfn.CONCAT( "Table of Water Quality of Produced Water and Flowback Water [",VLOOKUP("concentration",#REF!, 2, FALSE),"]")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -17324,9 +17038,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Initial Water Quality at Storage [", VLOOKUP("concentration", Units!A2:B9, 2, FALSE),,"]")</f>
-        <v>Table of Initial Water Quality at Storage [mg/liter]</v>
+      <c r="A1" s="1" t="e">
+        <f>_xlfn.CONCAT( "Table of Initial Water Quality at Storage [", VLOOKUP("concentration",#REF!, 2, FALSE),,"]")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -17373,9 +17087,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Initial Water Quality at Completions Pad Storage [",VLOOKUP("concentration", Units!$A$2:$B$11, 2, FALSE),"]")</f>
-        <v>Table of Initial Water Quality at Completions Pad Storage [mg/liter]</v>
+      <c r="A1" s="1" t="e">
+        <f>_xlfn.CONCAT( "Table of Initial Water Quality at Completions Pad Storage [",VLOOKUP("concentration",#REF!, 2, FALSE),"]")</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -17716,9 +17430,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Treatment Expansion Lead Time [",VLOOKUP("decision period", Units!$A$2:$B$11, 2, FALSE),"s]")</f>
-        <v>Table of Treatment Expansion Lead Time [weeks]</v>
+      <c r="A1" s="1" t="e">
+        <f>_xlfn.CONCAT( "Table of Treatment Expansion Lead Time [",VLOOKUP("decision period",#REF!, 2, FALSE),"s]")</f>
+        <v>#REF!</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -17843,9 +17557,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="str">
-        <f>_xlfn.CONCAT( "Table of Disposal Expansion Lead Time [",VLOOKUP("decision period", Units!$A$2:$B$11, 2, FALSE),"s]")</f>
-        <v>Table of Disposal Expansion Lead Time [weeks]</v>
+      <c r="A1" s="1" t="e">
+        <f>_xlfn.CONCAT( "Table of Disposal Expansion Lead Time [",VLOOKUP("decision period",#REF!, 2, FALSE),"s]")</f>
+        <v>#REF!</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>

</xml_diff>